<commit_message>
solved trendytech DSA Mod2
</commit_message>
<xml_diff>
--- a/LeetCode/Neetcode 150.xlsx
+++ b/LeetCode/Neetcode 150.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myWork\python\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29865BF1-FC4A-4612-A050-D9C47167698F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B403DEB-0D5B-47BC-AAFF-499709787929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,17 +20,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ARA Progress - Level 1'!$A$1:$X$732</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -1202,6 +1191,13 @@
           <c:val>
             <c:numRef>
               <c:f>'ARA Progress - Level 1'!$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>63</c:v>
+                </c:pt>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -1249,6 +1245,10 @@
           <c:val>
             <c:numRef>
               <c:f>'ARA Progress - Level 1'!$D$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -1679,14 +1679,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:X732"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+      <pane ySplit="2" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A123" sqref="A1:X732"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1741,7 +1741,7 @@
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
     </row>
-    <row r="2" spans="1:24" ht="12.75" hidden="1">
+    <row r="2" spans="1:24" ht="12.75">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1772,7 +1772,7 @@
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
     </row>
-    <row r="3" spans="1:24" ht="12.75" hidden="1">
+    <row r="3" spans="1:24" ht="12.75">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="12.75" hidden="1">
+    <row r="11" spans="1:24" ht="12.75">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:24" ht="12.75" hidden="1">
+    <row r="20" spans="1:24" ht="12.75">
       <c r="A20" s="8" t="s">
         <v>26</v>
       </c>
@@ -2044,7 +2044,7 @@
       <c r="D20" s="10"/>
       <c r="E20" s="11"/>
     </row>
-    <row r="21" spans="1:24" ht="12.75" hidden="1">
+    <row r="21" spans="1:24" ht="12.75">
       <c r="A21" s="8" t="s">
         <v>27</v>
       </c>
@@ -2085,7 +2085,7 @@
       </c>
       <c r="E23" s="11"/>
     </row>
-    <row r="24" spans="1:24" ht="12.75" hidden="1">
+    <row r="24" spans="1:24" ht="12.75">
       <c r="A24" s="8" t="s">
         <v>32</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="12.75" hidden="1">
+    <row r="28" spans="1:24" ht="12.75">
       <c r="A28" s="16" t="s">
         <v>37</v>
       </c>
@@ -2492,7 +2492,7 @@
       <c r="D52" s="10"/>
       <c r="E52" s="11"/>
     </row>
-    <row r="53" spans="1:6" ht="12.75" hidden="1">
+    <row r="53" spans="1:6" ht="12.75">
       <c r="A53" s="8" t="s">
         <v>63</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="12.75" hidden="1">
+    <row r="56" spans="1:6" ht="12.75">
       <c r="A56" s="8" t="s">
         <v>68</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="12.75" hidden="1">
+    <row r="59" spans="1:6" ht="12.75">
       <c r="A59" s="8" t="s">
         <v>71</v>
       </c>
@@ -2585,7 +2585,7 @@
       <c r="D59" s="10"/>
       <c r="E59" s="11"/>
     </row>
-    <row r="60" spans="1:6" ht="12.75" hidden="1">
+    <row r="60" spans="1:6" ht="12.75">
       <c r="A60" s="8" t="s">
         <v>72</v>
       </c>
@@ -2596,7 +2596,7 @@
       <c r="D60" s="10"/>
       <c r="E60" s="11"/>
     </row>
-    <row r="61" spans="1:6" ht="12.75" hidden="1">
+    <row r="61" spans="1:6" ht="12.75">
       <c r="A61" s="8" t="s">
         <v>73</v>
       </c>
@@ -2607,7 +2607,7 @@
       <c r="D61" s="10"/>
       <c r="E61" s="11"/>
     </row>
-    <row r="62" spans="1:6" ht="12.75" hidden="1">
+    <row r="62" spans="1:6" ht="12.75">
       <c r="A62" s="8" t="s">
         <v>74</v>
       </c>
@@ -2618,7 +2618,7 @@
       <c r="D62" s="10"/>
       <c r="E62" s="11"/>
     </row>
-    <row r="63" spans="1:6" ht="12.75" hidden="1">
+    <row r="63" spans="1:6" ht="12.75">
       <c r="A63" s="8" t="s">
         <v>75</v>
       </c>
@@ -2629,7 +2629,7 @@
       <c r="D63" s="10"/>
       <c r="E63" s="11"/>
     </row>
-    <row r="64" spans="1:6" ht="12.75" hidden="1">
+    <row r="64" spans="1:6" ht="12.75">
       <c r="A64" s="8" t="s">
         <v>76</v>
       </c>
@@ -2666,7 +2666,7 @@
       <c r="D66" s="10"/>
       <c r="E66" s="11"/>
     </row>
-    <row r="67" spans="1:24" ht="12.75" hidden="1">
+    <row r="67" spans="1:24" ht="12.75">
       <c r="A67" s="8" t="s">
         <v>79</v>
       </c>
@@ -2690,7 +2690,7 @@
       <c r="D68" s="10"/>
       <c r="E68" s="11"/>
     </row>
-    <row r="69" spans="1:24" ht="12.75" hidden="1">
+    <row r="69" spans="1:24" ht="12.75">
       <c r="A69" s="8" t="s">
         <v>81</v>
       </c>
@@ -2701,7 +2701,7 @@
       <c r="D69" s="10"/>
       <c r="E69" s="11"/>
     </row>
-    <row r="70" spans="1:24" ht="12.75" hidden="1">
+    <row r="70" spans="1:24" ht="12.75">
       <c r="A70" s="8" t="s">
         <v>82</v>
       </c>
@@ -2712,7 +2712,7 @@
       <c r="D70" s="10"/>
       <c r="E70" s="11"/>
     </row>
-    <row r="71" spans="1:24" ht="12.75" hidden="1">
+    <row r="71" spans="1:24" ht="12.75">
       <c r="A71" s="8" t="s">
         <v>83</v>
       </c>
@@ -2723,7 +2723,7 @@
       <c r="D71" s="10"/>
       <c r="E71" s="11"/>
     </row>
-    <row r="72" spans="1:24" ht="12.75" hidden="1">
+    <row r="72" spans="1:24" ht="12.75">
       <c r="A72" s="8" t="s">
         <v>84</v>
       </c>
@@ -2734,7 +2734,7 @@
       <c r="D72" s="10"/>
       <c r="E72" s="11"/>
     </row>
-    <row r="73" spans="1:24" ht="12.75" hidden="1">
+    <row r="73" spans="1:24" ht="12.75">
       <c r="A73" s="8" t="s">
         <v>85</v>
       </c>
@@ -2743,7 +2743,7 @@
       </c>
       <c r="E73" s="11"/>
     </row>
-    <row r="74" spans="1:24" ht="12.75" hidden="1">
+    <row r="74" spans="1:24" ht="12.75">
       <c r="A74" s="8" t="s">
         <v>86</v>
       </c>
@@ -2752,7 +2752,7 @@
       </c>
       <c r="E74" s="11"/>
     </row>
-    <row r="75" spans="1:24" ht="12.75" hidden="1">
+    <row r="75" spans="1:24" ht="12.75">
       <c r="A75" s="8" t="s">
         <v>87</v>
       </c>
@@ -2763,7 +2763,7 @@
       <c r="D75" s="10"/>
       <c r="E75" s="11"/>
     </row>
-    <row r="76" spans="1:24" ht="12.75" hidden="1">
+    <row r="76" spans="1:24" ht="12.75">
       <c r="A76" s="8" t="s">
         <v>88</v>
       </c>
@@ -2774,7 +2774,7 @@
       <c r="D76" s="10"/>
       <c r="E76" s="11"/>
     </row>
-    <row r="77" spans="1:24" ht="12.75" hidden="1">
+    <row r="77" spans="1:24" ht="12.75">
       <c r="A77" s="16" t="s">
         <v>90</v>
       </c>
@@ -2943,7 +2943,7 @@
       <c r="D88" s="10"/>
       <c r="E88" s="11"/>
     </row>
-    <row r="89" spans="1:24" ht="12.75" hidden="1">
+    <row r="89" spans="1:24" ht="12.75">
       <c r="A89" s="8" t="s">
         <v>102</v>
       </c>
@@ -2953,7 +2953,7 @@
       <c r="D89" s="10"/>
       <c r="E89" s="11"/>
     </row>
-    <row r="90" spans="1:24" ht="12.75" hidden="1">
+    <row r="90" spans="1:24" ht="12.75">
       <c r="A90" s="8" t="s">
         <v>103</v>
       </c>
@@ -2963,7 +2963,7 @@
       <c r="D90" s="10"/>
       <c r="E90" s="11"/>
     </row>
-    <row r="91" spans="1:24" ht="12.75" hidden="1">
+    <row r="91" spans="1:24" ht="12.75">
       <c r="A91" s="8" t="s">
         <v>104</v>
       </c>
@@ -2973,7 +2973,7 @@
       <c r="D91" s="10"/>
       <c r="E91" s="11"/>
     </row>
-    <row r="92" spans="1:24" ht="12.75" hidden="1">
+    <row r="92" spans="1:24" ht="12.75">
       <c r="A92" s="8" t="s">
         <v>105</v>
       </c>
@@ -2982,7 +2982,7 @@
       </c>
       <c r="E92" s="11"/>
     </row>
-    <row r="93" spans="1:24" ht="12.75" hidden="1">
+    <row r="93" spans="1:24" ht="12.75">
       <c r="A93" s="8" t="s">
         <v>106</v>
       </c>
@@ -2992,7 +2992,7 @@
       <c r="D93" s="10"/>
       <c r="E93" s="11"/>
     </row>
-    <row r="94" spans="1:24" ht="12.75" hidden="1">
+    <row r="94" spans="1:24" ht="12.75">
       <c r="A94" s="6" t="s">
         <v>107</v>
       </c>
@@ -3020,7 +3020,7 @@
       <c r="W94" s="7"/>
       <c r="X94" s="7"/>
     </row>
-    <row r="95" spans="1:24" ht="12.75" hidden="1">
+    <row r="95" spans="1:24" ht="12.75">
       <c r="A95" s="8" t="s">
         <v>108</v>
       </c>
@@ -3030,7 +3030,7 @@
       <c r="D95" s="10"/>
       <c r="E95" s="11"/>
     </row>
-    <row r="96" spans="1:24" ht="12.75" hidden="1">
+    <row r="96" spans="1:24" ht="12.75">
       <c r="A96" s="8" t="s">
         <v>109</v>
       </c>
@@ -3040,7 +3040,7 @@
       <c r="D96" s="10"/>
       <c r="E96" s="11"/>
     </row>
-    <row r="97" spans="1:24" ht="12.75" hidden="1">
+    <row r="97" spans="1:24" ht="12.75">
       <c r="A97" s="8" t="s">
         <v>110</v>
       </c>
@@ -3050,7 +3050,7 @@
       <c r="D97" s="10"/>
       <c r="E97" s="11"/>
     </row>
-    <row r="98" spans="1:24" ht="12.75" hidden="1">
+    <row r="98" spans="1:24" ht="12.75">
       <c r="A98" s="8" t="s">
         <v>111</v>
       </c>
@@ -3060,7 +3060,7 @@
       <c r="D98" s="10"/>
       <c r="E98" s="11"/>
     </row>
-    <row r="99" spans="1:24" ht="12.75" hidden="1">
+    <row r="99" spans="1:24" ht="12.75">
       <c r="A99" s="8" t="s">
         <v>112</v>
       </c>
@@ -3070,7 +3070,7 @@
       <c r="D99" s="10"/>
       <c r="E99" s="11"/>
     </row>
-    <row r="100" spans="1:24" ht="12.75" hidden="1">
+    <row r="100" spans="1:24" ht="12.75">
       <c r="A100" s="8" t="s">
         <v>113</v>
       </c>
@@ -3080,7 +3080,7 @@
       <c r="D100" s="10"/>
       <c r="E100" s="11"/>
     </row>
-    <row r="101" spans="1:24" ht="12.75" hidden="1">
+    <row r="101" spans="1:24" ht="12.75">
       <c r="A101" s="8" t="s">
         <v>114</v>
       </c>
@@ -3090,7 +3090,7 @@
       <c r="D101" s="10"/>
       <c r="E101" s="11"/>
     </row>
-    <row r="102" spans="1:24" ht="12.75" hidden="1">
+    <row r="102" spans="1:24" ht="12.75">
       <c r="A102" s="8" t="s">
         <v>115</v>
       </c>
@@ -3101,7 +3101,7 @@
       <c r="E102" s="11"/>
       <c r="K102" s="4"/>
     </row>
-    <row r="103" spans="1:24" ht="12.75" hidden="1">
+    <row r="103" spans="1:24" ht="12.75">
       <c r="A103" s="8" t="s">
         <v>116</v>
       </c>
@@ -3126,7 +3126,7 @@
       <c r="E104" s="11"/>
       <c r="K104" s="4"/>
     </row>
-    <row r="105" spans="1:24" ht="12.75" hidden="1">
+    <row r="105" spans="1:24" ht="12.75">
       <c r="A105" s="8" t="s">
         <v>118</v>
       </c>
@@ -3137,7 +3137,7 @@
       <c r="E105" s="11"/>
       <c r="K105" s="4"/>
     </row>
-    <row r="106" spans="1:24" ht="12.75" hidden="1">
+    <row r="106" spans="1:24" ht="12.75">
       <c r="A106" s="8" t="s">
         <v>119</v>
       </c>
@@ -3147,7 +3147,7 @@
       <c r="E106" s="11"/>
       <c r="K106" s="4"/>
     </row>
-    <row r="107" spans="1:24" ht="12.75" hidden="1">
+    <row r="107" spans="1:24" ht="12.75">
       <c r="A107" s="20" t="s">
         <v>120</v>
       </c>
@@ -3175,7 +3175,7 @@
       <c r="W107" s="13"/>
       <c r="X107" s="13"/>
     </row>
-    <row r="108" spans="1:24" ht="12.75" hidden="1">
+    <row r="108" spans="1:24" ht="12.75">
       <c r="A108" s="23" t="s">
         <v>121</v>
       </c>
@@ -3186,7 +3186,7 @@
       <c r="F108" s="11"/>
       <c r="K108" s="4"/>
     </row>
-    <row r="109" spans="1:24" ht="12.75" hidden="1">
+    <row r="109" spans="1:24" ht="12.75">
       <c r="A109" s="24" t="s">
         <v>122</v>
       </c>
@@ -3197,7 +3197,7 @@
       <c r="F109" s="11"/>
       <c r="K109" s="4"/>
     </row>
-    <row r="110" spans="1:24" ht="12.75" hidden="1">
+    <row r="110" spans="1:24" ht="12.75">
       <c r="A110" s="24" t="s">
         <v>123</v>
       </c>
@@ -3208,7 +3208,7 @@
       <c r="F110" s="11"/>
       <c r="K110" s="4"/>
     </row>
-    <row r="111" spans="1:24" ht="12.75" hidden="1">
+    <row r="111" spans="1:24" ht="12.75">
       <c r="A111" s="24" t="s">
         <v>124</v>
       </c>
@@ -3219,7 +3219,7 @@
       <c r="E111" s="11"/>
       <c r="K111" s="4"/>
     </row>
-    <row r="112" spans="1:24" ht="12.75" hidden="1">
+    <row r="112" spans="1:24" ht="12.75">
       <c r="A112" s="24" t="s">
         <v>125</v>
       </c>
@@ -3230,7 +3230,7 @@
       <c r="E112" s="11"/>
       <c r="K112" s="4"/>
     </row>
-    <row r="113" spans="1:24" ht="12.75" hidden="1">
+    <row r="113" spans="1:24" ht="12.75">
       <c r="A113" s="24" t="s">
         <v>126</v>
       </c>
@@ -3241,7 +3241,7 @@
       <c r="E113" s="11"/>
       <c r="K113" s="4"/>
     </row>
-    <row r="114" spans="1:24" ht="12.75" hidden="1">
+    <row r="114" spans="1:24" ht="12.75">
       <c r="A114" s="24" t="s">
         <v>127</v>
       </c>
@@ -3252,7 +3252,7 @@
       <c r="E114" s="11"/>
       <c r="K114" s="4"/>
     </row>
-    <row r="115" spans="1:24" ht="12.75" hidden="1">
+    <row r="115" spans="1:24" ht="12.75">
       <c r="A115" s="24" t="s">
         <v>128</v>
       </c>
@@ -3263,7 +3263,7 @@
       <c r="E115" s="11"/>
       <c r="K115" s="4"/>
     </row>
-    <row r="116" spans="1:24" ht="12.75" hidden="1">
+    <row r="116" spans="1:24" ht="12.75">
       <c r="A116" s="24" t="s">
         <v>129</v>
       </c>
@@ -3274,7 +3274,7 @@
       <c r="E116" s="11"/>
       <c r="K116" s="4"/>
     </row>
-    <row r="117" spans="1:24" ht="12.75" hidden="1">
+    <row r="117" spans="1:24" ht="12.75">
       <c r="A117" s="24" t="s">
         <v>130</v>
       </c>
@@ -3285,7 +3285,7 @@
       <c r="E117" s="11"/>
       <c r="K117" s="4"/>
     </row>
-    <row r="118" spans="1:24" ht="12.75" hidden="1">
+    <row r="118" spans="1:24" ht="12.75">
       <c r="A118" s="24" t="s">
         <v>131</v>
       </c>
@@ -3296,7 +3296,7 @@
       <c r="E118" s="11"/>
       <c r="K118" s="4"/>
     </row>
-    <row r="119" spans="1:24" ht="12.75" hidden="1">
+    <row r="119" spans="1:24" ht="12.75">
       <c r="A119" s="24" t="s">
         <v>132</v>
       </c>
@@ -3307,7 +3307,7 @@
       <c r="E119" s="11"/>
       <c r="K119" s="4"/>
     </row>
-    <row r="120" spans="1:24" ht="12.75" hidden="1">
+    <row r="120" spans="1:24" ht="12.75">
       <c r="A120" s="24" t="s">
         <v>133</v>
       </c>
@@ -3318,7 +3318,7 @@
       <c r="E120" s="11"/>
       <c r="K120" s="4"/>
     </row>
-    <row r="121" spans="1:24" ht="12.75" hidden="1">
+    <row r="121" spans="1:24" ht="12.75">
       <c r="A121" s="24" t="s">
         <v>134</v>
       </c>
@@ -3329,7 +3329,7 @@
       <c r="E121" s="11"/>
       <c r="K121" s="4"/>
     </row>
-    <row r="122" spans="1:24" ht="12.75" hidden="1">
+    <row r="122" spans="1:24" ht="12.75">
       <c r="A122" s="24" t="s">
         <v>135</v>
       </c>
@@ -3339,7 +3339,7 @@
       <c r="E122" s="11"/>
       <c r="K122" s="4"/>
     </row>
-    <row r="123" spans="1:24" ht="12.75" hidden="1">
+    <row r="123" spans="1:24" ht="12.75">
       <c r="A123" s="24" t="s">
         <v>136</v>
       </c>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="E123" s="11"/>
     </row>
-    <row r="124" spans="1:24" ht="12.75" hidden="1">
+    <row r="124" spans="1:24" ht="12.75">
       <c r="A124" s="24" t="s">
         <v>137</v>
       </c>
@@ -3358,7 +3358,7 @@
       <c r="D124" s="10"/>
       <c r="E124" s="11"/>
     </row>
-    <row r="125" spans="1:24" ht="12.75" hidden="1">
+    <row r="125" spans="1:24" ht="12.75">
       <c r="A125" s="20" t="s">
         <v>138</v>
       </c>
@@ -3386,7 +3386,7 @@
       <c r="W125" s="13"/>
       <c r="X125" s="13"/>
     </row>
-    <row r="126" spans="1:24" ht="12.75" hidden="1">
+    <row r="126" spans="1:24" ht="12.75">
       <c r="A126" s="23" t="s">
         <v>138</v>
       </c>
@@ -3409,7 +3409,7 @@
       <c r="D127" s="10"/>
       <c r="E127" s="11"/>
     </row>
-    <row r="128" spans="1:24" ht="12.75" hidden="1">
+    <row r="128" spans="1:24" ht="12.75">
       <c r="A128" s="24" t="s">
         <v>140</v>
       </c>
@@ -3419,7 +3419,7 @@
       <c r="D128" s="10"/>
       <c r="E128" s="11"/>
     </row>
-    <row r="129" spans="1:5" ht="12.75" hidden="1">
+    <row r="129" spans="1:5" ht="12.75">
       <c r="A129" s="24" t="s">
         <v>141</v>
       </c>
@@ -3429,7 +3429,7 @@
       <c r="D129" s="10"/>
       <c r="E129" s="11"/>
     </row>
-    <row r="130" spans="1:5" ht="12.75" hidden="1">
+    <row r="130" spans="1:5" ht="12.75">
       <c r="A130" s="24" t="s">
         <v>142</v>
       </c>
@@ -3439,7 +3439,7 @@
       <c r="D130" s="10"/>
       <c r="E130" s="11"/>
     </row>
-    <row r="131" spans="1:5" ht="12.75" hidden="1">
+    <row r="131" spans="1:5" ht="12.75">
       <c r="A131" s="24" t="s">
         <v>143</v>
       </c>
@@ -3449,7 +3449,7 @@
       <c r="D131" s="10"/>
       <c r="E131" s="11"/>
     </row>
-    <row r="132" spans="1:5" ht="12.75" hidden="1">
+    <row r="132" spans="1:5" ht="12.75">
       <c r="A132" s="24" t="s">
         <v>144</v>
       </c>
@@ -3459,7 +3459,7 @@
       <c r="D132" s="10"/>
       <c r="E132" s="11"/>
     </row>
-    <row r="133" spans="1:5" ht="12.75" hidden="1">
+    <row r="133" spans="1:5" ht="12.75">
       <c r="A133" s="24" t="s">
         <v>145</v>
       </c>
@@ -3469,7 +3469,7 @@
       <c r="D133" s="10"/>
       <c r="E133" s="11"/>
     </row>
-    <row r="134" spans="1:5" ht="12.75" hidden="1">
+    <row r="134" spans="1:5" ht="12.75">
       <c r="A134" s="24" t="s">
         <v>146</v>
       </c>
@@ -3479,7 +3479,7 @@
       <c r="D134" s="10"/>
       <c r="E134" s="11"/>
     </row>
-    <row r="135" spans="1:5" ht="12.75" hidden="1">
+    <row r="135" spans="1:5" ht="12.75">
       <c r="A135" s="24" t="s">
         <v>147</v>
       </c>
@@ -3489,7 +3489,7 @@
       <c r="D135" s="10"/>
       <c r="E135" s="11"/>
     </row>
-    <row r="136" spans="1:5" ht="12.75" hidden="1">
+    <row r="136" spans="1:5" ht="12.75">
       <c r="A136" s="24" t="s">
         <v>148</v>
       </c>
@@ -3499,7 +3499,7 @@
       <c r="D136" s="10"/>
       <c r="E136" s="11"/>
     </row>
-    <row r="137" spans="1:5" ht="12.75" hidden="1">
+    <row r="137" spans="1:5" ht="12.75">
       <c r="A137" s="24" t="s">
         <v>149</v>
       </c>
@@ -3509,7 +3509,7 @@
       <c r="D137" s="10"/>
       <c r="E137" s="11"/>
     </row>
-    <row r="138" spans="1:5" ht="12.75" hidden="1">
+    <row r="138" spans="1:5" ht="12.75">
       <c r="A138" s="24" t="s">
         <v>150</v>
       </c>
@@ -3519,7 +3519,7 @@
       <c r="D138" s="10"/>
       <c r="E138" s="11"/>
     </row>
-    <row r="139" spans="1:5" ht="12.75" hidden="1">
+    <row r="139" spans="1:5" ht="12.75">
       <c r="A139" s="24" t="s">
         <v>151</v>
       </c>
@@ -3529,7 +3529,7 @@
       <c r="D139" s="10"/>
       <c r="E139" s="11"/>
     </row>
-    <row r="140" spans="1:5" ht="12.75" hidden="1">
+    <row r="140" spans="1:5" ht="12.75">
       <c r="A140" s="24" t="s">
         <v>152</v>
       </c>
@@ -3539,7 +3539,7 @@
       <c r="D140" s="10"/>
       <c r="E140" s="11"/>
     </row>
-    <row r="141" spans="1:5" ht="12.75" hidden="1">
+    <row r="141" spans="1:5" ht="12.75">
       <c r="A141" s="24" t="s">
         <v>153</v>
       </c>
@@ -3549,7 +3549,7 @@
       <c r="D141" s="10"/>
       <c r="E141" s="11"/>
     </row>
-    <row r="142" spans="1:5" ht="12.75" hidden="1">
+    <row r="142" spans="1:5" ht="12.75">
       <c r="A142" s="24" t="s">
         <v>154</v>
       </c>
@@ -3559,102 +3559,102 @@
       <c r="D142" s="10"/>
       <c r="E142" s="11"/>
     </row>
-    <row r="143" spans="1:5" ht="12.75" hidden="1">
+    <row r="143" spans="1:5" ht="12.75">
       <c r="A143" s="19"/>
       <c r="B143" s="19"/>
       <c r="D143" s="10"/>
       <c r="E143" s="11"/>
     </row>
-    <row r="144" spans="1:5" ht="12.75" hidden="1">
+    <row r="144" spans="1:5" ht="12.75">
       <c r="A144" s="19"/>
       <c r="B144" s="19"/>
       <c r="D144" s="10"/>
       <c r="E144" s="11"/>
     </row>
-    <row r="145" spans="1:24" ht="12.75" hidden="1">
+    <row r="145" spans="1:24" ht="12.75">
       <c r="A145" s="19"/>
       <c r="B145" s="19"/>
       <c r="D145" s="10"/>
       <c r="E145" s="11"/>
     </row>
-    <row r="146" spans="1:24" ht="12.75" hidden="1">
+    <row r="146" spans="1:24" ht="12.75">
       <c r="A146" s="19"/>
       <c r="B146" s="19"/>
       <c r="D146" s="10"/>
       <c r="E146" s="11"/>
     </row>
-    <row r="147" spans="1:24" ht="12.75" hidden="1">
+    <row r="147" spans="1:24" ht="12.75">
       <c r="A147" s="19"/>
       <c r="B147" s="19"/>
       <c r="D147" s="10"/>
       <c r="E147" s="11"/>
     </row>
-    <row r="148" spans="1:24" ht="12.75" hidden="1">
+    <row r="148" spans="1:24" ht="12.75">
       <c r="A148" s="19"/>
       <c r="B148" s="19"/>
       <c r="D148" s="10"/>
       <c r="E148" s="11"/>
     </row>
-    <row r="149" spans="1:24" ht="12.75" hidden="1">
+    <row r="149" spans="1:24" ht="12.75">
       <c r="A149" s="19"/>
       <c r="B149" s="19"/>
       <c r="D149" s="10"/>
       <c r="E149" s="11"/>
     </row>
-    <row r="150" spans="1:24" ht="12.75" hidden="1">
+    <row r="150" spans="1:24" ht="12.75">
       <c r="A150" s="19"/>
       <c r="B150" s="19"/>
       <c r="D150" s="10"/>
       <c r="E150" s="11"/>
     </row>
-    <row r="151" spans="1:24" ht="12.75" hidden="1">
+    <row r="151" spans="1:24" ht="12.75">
       <c r="A151" s="19"/>
       <c r="B151" s="19"/>
       <c r="D151" s="10"/>
       <c r="E151" s="11"/>
     </row>
-    <row r="152" spans="1:24" ht="12.75" hidden="1">
+    <row r="152" spans="1:24" ht="12.75">
       <c r="A152" s="19"/>
       <c r="B152" s="19"/>
       <c r="D152" s="10"/>
       <c r="E152" s="11"/>
     </row>
-    <row r="153" spans="1:24" ht="12.75" hidden="1">
+    <row r="153" spans="1:24" ht="12.75">
       <c r="A153" s="19"/>
       <c r="B153" s="19"/>
       <c r="D153" s="10"/>
       <c r="E153" s="11"/>
     </row>
-    <row r="154" spans="1:24" ht="12.75" hidden="1">
+    <row r="154" spans="1:24" ht="12.75">
       <c r="A154" s="19"/>
       <c r="B154" s="19"/>
       <c r="D154" s="10"/>
       <c r="E154" s="11"/>
     </row>
-    <row r="155" spans="1:24" ht="12.75" hidden="1">
+    <row r="155" spans="1:24" ht="12.75">
       <c r="A155" s="19"/>
       <c r="B155" s="19"/>
       <c r="D155" s="10"/>
       <c r="E155" s="11"/>
     </row>
-    <row r="156" spans="1:24" ht="12.75" hidden="1">
+    <row r="156" spans="1:24" ht="12.75">
       <c r="A156" s="19"/>
       <c r="B156" s="19"/>
       <c r="D156" s="10"/>
       <c r="E156" s="11"/>
     </row>
-    <row r="157" spans="1:24" ht="12.75" hidden="1">
+    <row r="157" spans="1:24" ht="12.75">
       <c r="A157" s="19"/>
       <c r="B157" s="19"/>
       <c r="D157" s="10"/>
       <c r="E157" s="11"/>
     </row>
-    <row r="158" spans="1:24" ht="12.75" hidden="1">
+    <row r="158" spans="1:24" ht="12.75">
       <c r="A158" s="19"/>
       <c r="B158" s="19"/>
       <c r="E158" s="11"/>
     </row>
-    <row r="159" spans="1:24" ht="12.75" hidden="1">
+    <row r="159" spans="1:24" ht="12.75">
       <c r="A159" s="6"/>
       <c r="B159" s="6"/>
       <c r="C159" s="13"/>
@@ -3680,119 +3680,119 @@
       <c r="W159" s="7"/>
       <c r="X159" s="7"/>
     </row>
-    <row r="160" spans="1:24" ht="12.75" hidden="1">
+    <row r="160" spans="1:24" ht="12.75">
       <c r="D160" s="10"/>
       <c r="E160" s="11"/>
     </row>
-    <row r="161" spans="1:7" ht="12.75" hidden="1">
+    <row r="161" spans="1:7" ht="12.75">
       <c r="D161" s="10"/>
       <c r="E161" s="11"/>
     </row>
-    <row r="162" spans="1:7" ht="12.75" hidden="1">
+    <row r="162" spans="1:7" ht="12.75">
       <c r="D162" s="10"/>
       <c r="E162" s="11"/>
     </row>
-    <row r="163" spans="1:7" ht="12.75" hidden="1">
+    <row r="163" spans="1:7" ht="12.75">
       <c r="D163" s="10"/>
       <c r="E163" s="11"/>
     </row>
-    <row r="164" spans="1:7" ht="12.75" hidden="1">
+    <row r="164" spans="1:7" ht="12.75">
       <c r="D164" s="10"/>
       <c r="E164" s="11"/>
     </row>
-    <row r="165" spans="1:7" ht="12.75" hidden="1">
+    <row r="165" spans="1:7" ht="12.75">
       <c r="A165" s="26"/>
       <c r="B165" s="26"/>
       <c r="D165" s="10"/>
       <c r="E165" s="11"/>
     </row>
-    <row r="166" spans="1:7" ht="12.75" hidden="1">
+    <row r="166" spans="1:7" ht="12.75">
       <c r="A166" s="26"/>
       <c r="B166" s="26"/>
       <c r="D166" s="10"/>
       <c r="E166" s="11"/>
     </row>
-    <row r="167" spans="1:7" ht="12.75" hidden="1">
+    <row r="167" spans="1:7" ht="12.75">
       <c r="A167" s="26"/>
       <c r="B167" s="26"/>
       <c r="D167" s="10"/>
       <c r="E167" s="11"/>
     </row>
-    <row r="168" spans="1:7" ht="12.75" hidden="1">
+    <row r="168" spans="1:7" ht="12.75">
       <c r="A168" s="26"/>
       <c r="B168" s="26"/>
       <c r="D168" s="10"/>
       <c r="E168" s="11"/>
     </row>
-    <row r="169" spans="1:7" ht="12.75" hidden="1">
+    <row r="169" spans="1:7" ht="12.75">
       <c r="A169" s="26"/>
       <c r="B169" s="26"/>
       <c r="D169" s="10"/>
       <c r="E169" s="11"/>
     </row>
-    <row r="170" spans="1:7" ht="12.75" hidden="1">
+    <row r="170" spans="1:7" ht="12.75">
       <c r="A170" s="26"/>
       <c r="B170" s="26"/>
       <c r="D170" s="10"/>
       <c r="E170" s="11"/>
     </row>
-    <row r="171" spans="1:7" ht="12.75" hidden="1">
+    <row r="171" spans="1:7" ht="12.75">
       <c r="A171" s="26"/>
       <c r="B171" s="26"/>
       <c r="D171" s="10"/>
       <c r="E171" s="11"/>
     </row>
-    <row r="172" spans="1:7" ht="12.75" hidden="1">
+    <row r="172" spans="1:7" ht="12.75">
       <c r="A172" s="26"/>
       <c r="B172" s="26"/>
       <c r="D172" s="10"/>
       <c r="E172" s="11"/>
     </row>
-    <row r="173" spans="1:7" ht="12.75" hidden="1">
+    <row r="173" spans="1:7" ht="12.75">
       <c r="A173" s="26"/>
       <c r="B173" s="26"/>
       <c r="D173" s="10"/>
       <c r="E173" s="11"/>
     </row>
-    <row r="174" spans="1:7" ht="12.75" hidden="1">
+    <row r="174" spans="1:7" ht="12.75">
       <c r="A174" s="26"/>
       <c r="B174" s="26"/>
       <c r="D174" s="10"/>
       <c r="E174" s="11"/>
     </row>
-    <row r="175" spans="1:7" ht="12.75" hidden="1">
+    <row r="175" spans="1:7" ht="12.75">
       <c r="A175" s="26"/>
       <c r="B175" s="26"/>
       <c r="D175" s="10"/>
       <c r="E175" s="11"/>
       <c r="G175" s="27"/>
     </row>
-    <row r="176" spans="1:7" ht="12.75" hidden="1">
+    <row r="176" spans="1:7" ht="12.75">
       <c r="A176" s="26"/>
       <c r="B176" s="26"/>
       <c r="D176" s="10"/>
       <c r="E176" s="11"/>
     </row>
-    <row r="177" spans="1:24" ht="12.75" hidden="1">
+    <row r="177" spans="1:24" ht="12.75">
       <c r="A177" s="26"/>
       <c r="B177" s="26"/>
       <c r="D177" s="10"/>
       <c r="E177" s="11"/>
     </row>
-    <row r="178" spans="1:24" ht="12.75" hidden="1">
+    <row r="178" spans="1:24" ht="12.75">
       <c r="A178" s="26"/>
       <c r="B178" s="26"/>
       <c r="D178" s="10"/>
       <c r="E178" s="11"/>
     </row>
-    <row r="179" spans="1:24" ht="12.75" hidden="1">
+    <row r="179" spans="1:24" ht="12.75">
       <c r="D179" s="10"/>
       <c r="E179" s="11"/>
     </row>
-    <row r="180" spans="1:24" ht="12.75" hidden="1">
+    <row r="180" spans="1:24" ht="12.75">
       <c r="E180" s="11"/>
     </row>
-    <row r="181" spans="1:24" ht="12.75" hidden="1">
+    <row r="181" spans="1:24" ht="12.75">
       <c r="A181" s="6"/>
       <c r="B181" s="6"/>
       <c r="C181" s="13"/>
@@ -3818,54 +3818,54 @@
       <c r="W181" s="7"/>
       <c r="X181" s="7"/>
     </row>
-    <row r="182" spans="1:24" ht="12.75" hidden="1">
+    <row r="182" spans="1:24" ht="12.75">
       <c r="A182" s="19"/>
       <c r="B182" s="19"/>
       <c r="D182" s="10"/>
       <c r="E182" s="11"/>
     </row>
-    <row r="183" spans="1:24" ht="12.75" hidden="1">
+    <row r="183" spans="1:24" ht="12.75">
       <c r="D183" s="10"/>
       <c r="E183" s="11"/>
     </row>
-    <row r="184" spans="1:24" ht="12.75" hidden="1">
+    <row r="184" spans="1:24" ht="12.75">
       <c r="D184" s="10"/>
       <c r="E184" s="11"/>
     </row>
-    <row r="185" spans="1:24" ht="12.75" hidden="1">
+    <row r="185" spans="1:24" ht="12.75">
       <c r="D185" s="10"/>
       <c r="E185" s="11"/>
     </row>
-    <row r="186" spans="1:24" ht="12.75" hidden="1">
+    <row r="186" spans="1:24" ht="12.75">
       <c r="D186" s="10"/>
       <c r="E186" s="11"/>
     </row>
-    <row r="187" spans="1:24" ht="12.75" hidden="1">
+    <row r="187" spans="1:24" ht="12.75">
       <c r="D187" s="10"/>
       <c r="E187" s="11"/>
     </row>
-    <row r="188" spans="1:24" ht="12.75" hidden="1">
+    <row r="188" spans="1:24" ht="12.75">
       <c r="D188" s="10"/>
       <c r="E188" s="11"/>
     </row>
-    <row r="189" spans="1:24" ht="12.75" hidden="1">
+    <row r="189" spans="1:24" ht="12.75">
       <c r="D189" s="10"/>
       <c r="E189" s="11"/>
     </row>
-    <row r="190" spans="1:24" ht="12.75" hidden="1">
+    <row r="190" spans="1:24" ht="12.75">
       <c r="D190" s="10"/>
       <c r="E190" s="11"/>
     </row>
-    <row r="191" spans="1:24" ht="12.75" hidden="1">
+    <row r="191" spans="1:24" ht="12.75">
       <c r="A191" s="25"/>
       <c r="B191" s="25"/>
       <c r="D191" s="10"/>
       <c r="E191" s="11"/>
     </row>
-    <row r="192" spans="1:24" ht="12.75" hidden="1">
+    <row r="192" spans="1:24" ht="12.75">
       <c r="E192" s="11"/>
     </row>
-    <row r="193" spans="1:24" ht="12.75" hidden="1">
+    <row r="193" spans="1:24" ht="12.75">
       <c r="A193" s="6"/>
       <c r="B193" s="6"/>
       <c r="C193" s="13"/>
@@ -3891,95 +3891,95 @@
       <c r="W193" s="7"/>
       <c r="X193" s="7"/>
     </row>
-    <row r="194" spans="1:24" ht="12.75" hidden="1">
+    <row r="194" spans="1:24" ht="12.75">
       <c r="A194" s="28"/>
       <c r="B194" s="28"/>
       <c r="D194" s="10"/>
       <c r="E194" s="11"/>
     </row>
-    <row r="195" spans="1:24" ht="12.75" hidden="1">
+    <row r="195" spans="1:24" ht="12.75">
       <c r="A195" s="29"/>
       <c r="B195" s="29"/>
       <c r="D195" s="10"/>
       <c r="E195" s="11"/>
     </row>
-    <row r="196" spans="1:24" ht="12.75" hidden="1">
+    <row r="196" spans="1:24" ht="12.75">
       <c r="A196" s="29"/>
       <c r="B196" s="29"/>
       <c r="D196" s="10"/>
       <c r="E196" s="11"/>
     </row>
-    <row r="197" spans="1:24" ht="12.75" hidden="1">
+    <row r="197" spans="1:24" ht="12.75">
       <c r="A197" s="29"/>
       <c r="B197" s="29"/>
       <c r="D197" s="10"/>
       <c r="E197" s="11"/>
     </row>
-    <row r="198" spans="1:24" ht="12.75" hidden="1">
+    <row r="198" spans="1:24" ht="12.75">
       <c r="A198" s="29"/>
       <c r="B198" s="29"/>
       <c r="D198" s="10"/>
       <c r="E198" s="11"/>
     </row>
-    <row r="199" spans="1:24" ht="12.75" hidden="1">
+    <row r="199" spans="1:24" ht="12.75">
       <c r="A199" s="29"/>
       <c r="B199" s="29"/>
       <c r="D199" s="10"/>
       <c r="E199" s="11"/>
     </row>
-    <row r="200" spans="1:24" ht="12.75" hidden="1">
+    <row r="200" spans="1:24" ht="12.75">
       <c r="A200" s="29"/>
       <c r="B200" s="29"/>
       <c r="D200" s="10"/>
       <c r="E200" s="11"/>
     </row>
-    <row r="201" spans="1:24" ht="12.75" hidden="1">
+    <row r="201" spans="1:24" ht="12.75">
       <c r="A201" s="29"/>
       <c r="B201" s="29"/>
       <c r="E201" s="11"/>
     </row>
-    <row r="202" spans="1:24" ht="12.75" hidden="1">
+    <row r="202" spans="1:24" ht="12.75">
       <c r="A202" s="29"/>
       <c r="B202" s="29"/>
       <c r="D202" s="10"/>
       <c r="E202" s="11"/>
     </row>
-    <row r="203" spans="1:24" ht="12.75" hidden="1">
+    <row r="203" spans="1:24" ht="12.75">
       <c r="A203" s="29"/>
       <c r="B203" s="29"/>
       <c r="D203" s="10"/>
       <c r="E203" s="11"/>
     </row>
-    <row r="204" spans="1:24" ht="12.75" hidden="1">
+    <row r="204" spans="1:24" ht="12.75">
       <c r="A204" s="29"/>
       <c r="B204" s="29"/>
       <c r="D204" s="10"/>
       <c r="E204" s="11"/>
     </row>
-    <row r="205" spans="1:24" ht="12.75" hidden="1">
+    <row r="205" spans="1:24" ht="12.75">
       <c r="A205" s="29"/>
       <c r="B205" s="29"/>
       <c r="D205" s="10"/>
       <c r="E205" s="11"/>
     </row>
-    <row r="206" spans="1:24" ht="12.75" hidden="1">
+    <row r="206" spans="1:24" ht="12.75">
       <c r="A206" s="29"/>
       <c r="B206" s="29"/>
       <c r="D206" s="10"/>
       <c r="E206" s="11"/>
     </row>
-    <row r="207" spans="1:24" ht="12.75" hidden="1">
+    <row r="207" spans="1:24" ht="12.75">
       <c r="A207" s="29"/>
       <c r="B207" s="29"/>
       <c r="D207" s="10"/>
       <c r="E207" s="11"/>
     </row>
-    <row r="208" spans="1:24" ht="12.75" hidden="1">
+    <row r="208" spans="1:24" ht="12.75">
       <c r="A208" s="29"/>
       <c r="B208" s="29"/>
       <c r="E208" s="11"/>
     </row>
-    <row r="209" spans="1:24" ht="12.75" hidden="1">
+    <row r="209" spans="1:24" ht="12.75">
       <c r="A209" s="30"/>
       <c r="B209" s="30"/>
       <c r="C209" s="13"/>
@@ -4005,2647 +4005,2641 @@
       <c r="W209" s="6"/>
       <c r="X209" s="6"/>
     </row>
-    <row r="210" spans="1:24" ht="12.75" hidden="1">
+    <row r="210" spans="1:24" ht="12.75">
       <c r="A210" s="29"/>
       <c r="B210" s="29"/>
       <c r="D210" s="10"/>
       <c r="E210" s="11"/>
     </row>
-    <row r="211" spans="1:24" ht="12.75" hidden="1">
+    <row r="211" spans="1:24" ht="12.75">
       <c r="A211" s="29"/>
       <c r="B211" s="29"/>
       <c r="D211" s="10"/>
       <c r="E211" s="11"/>
     </row>
-    <row r="212" spans="1:24" ht="12.75" hidden="1">
+    <row r="212" spans="1:24" ht="12.75">
       <c r="A212" s="29"/>
       <c r="B212" s="29"/>
       <c r="D212" s="10"/>
       <c r="E212" s="11"/>
     </row>
-    <row r="213" spans="1:24" ht="12.75" hidden="1">
+    <row r="213" spans="1:24" ht="12.75">
       <c r="A213" s="29"/>
       <c r="B213" s="29"/>
       <c r="D213" s="10"/>
       <c r="E213" s="11"/>
     </row>
-    <row r="214" spans="1:24" ht="12.75" hidden="1">
+    <row r="214" spans="1:24" ht="12.75">
       <c r="A214" s="29"/>
       <c r="B214" s="29"/>
       <c r="D214" s="10"/>
       <c r="E214" s="11"/>
     </row>
-    <row r="215" spans="1:24" ht="12.75" hidden="1">
+    <row r="215" spans="1:24" ht="12.75">
       <c r="A215" s="29"/>
       <c r="B215" s="29"/>
       <c r="D215" s="10"/>
       <c r="E215" s="11"/>
     </row>
-    <row r="216" spans="1:24" ht="12.75" hidden="1">
+    <row r="216" spans="1:24" ht="12.75">
       <c r="A216" s="29"/>
       <c r="B216" s="29"/>
       <c r="D216" s="10"/>
       <c r="E216" s="11"/>
     </row>
-    <row r="217" spans="1:24" ht="12.75" hidden="1">
+    <row r="217" spans="1:24" ht="12.75">
       <c r="A217" s="29"/>
       <c r="B217" s="29"/>
       <c r="D217" s="10"/>
       <c r="E217" s="11"/>
     </row>
-    <row r="218" spans="1:24" ht="12.75" hidden="1">
+    <row r="218" spans="1:24" ht="12.75">
       <c r="A218" s="29"/>
       <c r="B218" s="29"/>
       <c r="D218" s="10"/>
       <c r="E218" s="11"/>
     </row>
-    <row r="219" spans="1:24" ht="12.75" hidden="1">
+    <row r="219" spans="1:24" ht="12.75">
       <c r="A219" s="29"/>
       <c r="B219" s="29"/>
       <c r="D219" s="10"/>
       <c r="E219" s="11"/>
     </row>
-    <row r="220" spans="1:24" ht="12.75" hidden="1">
+    <row r="220" spans="1:24" ht="12.75">
       <c r="A220" s="29"/>
       <c r="B220" s="29"/>
       <c r="D220" s="10"/>
       <c r="E220" s="11"/>
     </row>
-    <row r="221" spans="1:24" ht="12.75" hidden="1">
+    <row r="221" spans="1:24" ht="12.75">
       <c r="A221" s="29"/>
       <c r="B221" s="29"/>
       <c r="D221" s="10"/>
       <c r="E221" s="11"/>
     </row>
-    <row r="222" spans="1:24" ht="12.75" hidden="1">
+    <row r="222" spans="1:24" ht="12.75">
       <c r="A222" s="29"/>
       <c r="B222" s="29"/>
       <c r="D222" s="10"/>
       <c r="E222" s="11"/>
     </row>
-    <row r="223" spans="1:24" ht="12.75" hidden="1">
+    <row r="223" spans="1:24" ht="12.75">
       <c r="A223" s="29"/>
       <c r="B223" s="29"/>
       <c r="D223" s="10"/>
       <c r="E223" s="11"/>
     </row>
-    <row r="224" spans="1:24" ht="12.75" hidden="1">
+    <row r="224" spans="1:24" ht="12.75">
       <c r="A224" s="29"/>
       <c r="B224" s="29"/>
       <c r="D224" s="10"/>
       <c r="E224" s="11"/>
     </row>
-    <row r="225" spans="1:5" ht="12.75" hidden="1">
+    <row r="225" spans="1:5" ht="12.75">
       <c r="A225" s="29"/>
       <c r="B225" s="29"/>
       <c r="D225" s="10"/>
       <c r="E225" s="11"/>
     </row>
-    <row r="226" spans="1:5" ht="12.75" hidden="1">
+    <row r="226" spans="1:5" ht="12.75">
       <c r="A226" s="29"/>
       <c r="B226" s="29"/>
       <c r="D226" s="10"/>
       <c r="E226" s="11"/>
     </row>
-    <row r="227" spans="1:5" ht="12.75" hidden="1">
+    <row r="227" spans="1:5" ht="12.75">
       <c r="A227" s="31"/>
       <c r="B227" s="31"/>
       <c r="D227" s="10"/>
       <c r="E227" s="11"/>
     </row>
-    <row r="228" spans="1:5" ht="12.75" hidden="1">
+    <row r="228" spans="1:5" ht="12.75">
       <c r="A228" s="29"/>
       <c r="B228" s="29"/>
       <c r="E228" s="11"/>
     </row>
-    <row r="229" spans="1:5" ht="12.75" hidden="1">
+    <row r="229" spans="1:5" ht="12.75">
       <c r="A229" s="29"/>
       <c r="B229" s="29"/>
       <c r="E229" s="11"/>
     </row>
-    <row r="230" spans="1:5" ht="12.75" hidden="1">
+    <row r="230" spans="1:5" ht="12.75">
       <c r="A230" s="29"/>
       <c r="B230" s="29"/>
       <c r="E230" s="11"/>
     </row>
-    <row r="231" spans="1:5" ht="12.75" hidden="1">
+    <row r="231" spans="1:5" ht="12.75">
       <c r="A231" s="10"/>
       <c r="B231" s="10"/>
       <c r="E231" s="11"/>
     </row>
-    <row r="232" spans="1:5" ht="12.75" hidden="1">
+    <row r="232" spans="1:5" ht="12.75">
       <c r="A232" s="10"/>
       <c r="B232" s="10"/>
       <c r="E232" s="11"/>
     </row>
-    <row r="233" spans="1:5" ht="12.75" hidden="1">
+    <row r="233" spans="1:5" ht="12.75">
       <c r="A233" s="10"/>
       <c r="B233" s="10"/>
       <c r="E233" s="11"/>
     </row>
-    <row r="234" spans="1:5" ht="12.75" hidden="1">
+    <row r="234" spans="1:5" ht="12.75">
       <c r="A234" s="10"/>
       <c r="B234" s="10"/>
       <c r="E234" s="11"/>
     </row>
-    <row r="235" spans="1:5" ht="12.75" hidden="1">
+    <row r="235" spans="1:5" ht="12.75">
       <c r="A235" s="10"/>
       <c r="B235" s="10"/>
       <c r="E235" s="11"/>
     </row>
-    <row r="236" spans="1:5" ht="12.75" hidden="1">
+    <row r="236" spans="1:5" ht="12.75">
       <c r="A236" s="10"/>
       <c r="B236" s="10"/>
       <c r="E236" s="11"/>
     </row>
-    <row r="237" spans="1:5" ht="12.75" hidden="1">
+    <row r="237" spans="1:5" ht="12.75">
       <c r="A237" s="10"/>
       <c r="B237" s="10"/>
       <c r="E237" s="11"/>
     </row>
-    <row r="238" spans="1:5" ht="12.75" hidden="1">
+    <row r="238" spans="1:5" ht="12.75">
       <c r="A238" s="10"/>
       <c r="B238" s="10"/>
       <c r="E238" s="11"/>
     </row>
-    <row r="239" spans="1:5" ht="12.75" hidden="1">
+    <row r="239" spans="1:5" ht="12.75">
       <c r="A239" s="10"/>
       <c r="B239" s="10"/>
       <c r="E239" s="11"/>
     </row>
-    <row r="240" spans="1:5" ht="12.75" hidden="1">
+    <row r="240" spans="1:5" ht="12.75">
       <c r="A240" s="10"/>
       <c r="B240" s="10"/>
       <c r="E240" s="11"/>
     </row>
-    <row r="241" spans="1:5" ht="12.75" hidden="1">
+    <row r="241" spans="1:5" ht="12.75">
       <c r="A241" s="10"/>
       <c r="B241" s="10"/>
       <c r="E241" s="11"/>
     </row>
-    <row r="242" spans="1:5" ht="12.75" hidden="1">
+    <row r="242" spans="1:5" ht="12.75">
       <c r="A242" s="10"/>
       <c r="B242" s="10"/>
       <c r="E242" s="11"/>
     </row>
-    <row r="243" spans="1:5" ht="12.75" hidden="1">
+    <row r="243" spans="1:5" ht="12.75">
       <c r="A243" s="10"/>
       <c r="B243" s="10"/>
       <c r="E243" s="11"/>
     </row>
-    <row r="244" spans="1:5" ht="12.75" hidden="1">
+    <row r="244" spans="1:5" ht="12.75">
       <c r="A244" s="10"/>
       <c r="B244" s="10"/>
       <c r="E244" s="11"/>
     </row>
-    <row r="245" spans="1:5" ht="12.75" hidden="1">
+    <row r="245" spans="1:5" ht="12.75">
       <c r="A245" s="10"/>
       <c r="B245" s="10"/>
       <c r="E245" s="11"/>
     </row>
-    <row r="246" spans="1:5" ht="12.75" hidden="1">
+    <row r="246" spans="1:5" ht="12.75">
       <c r="A246" s="10"/>
       <c r="B246" s="10"/>
       <c r="E246" s="11"/>
     </row>
-    <row r="247" spans="1:5" ht="12.75" hidden="1">
+    <row r="247" spans="1:5" ht="12.75">
       <c r="A247" s="10"/>
       <c r="B247" s="10"/>
       <c r="E247" s="11"/>
     </row>
-    <row r="248" spans="1:5" ht="12.75" hidden="1">
+    <row r="248" spans="1:5" ht="12.75">
       <c r="A248" s="10"/>
       <c r="B248" s="10"/>
       <c r="E248" s="11"/>
     </row>
-    <row r="249" spans="1:5" ht="12.75" hidden="1">
+    <row r="249" spans="1:5" ht="12.75">
       <c r="A249" s="10"/>
       <c r="B249" s="10"/>
       <c r="E249" s="11"/>
     </row>
-    <row r="250" spans="1:5" ht="12.75" hidden="1">
+    <row r="250" spans="1:5" ht="12.75">
       <c r="A250" s="10"/>
       <c r="B250" s="10"/>
       <c r="E250" s="11"/>
     </row>
-    <row r="251" spans="1:5" ht="12.75" hidden="1">
+    <row r="251" spans="1:5" ht="12.75">
       <c r="A251" s="10"/>
       <c r="B251" s="10"/>
       <c r="E251" s="11"/>
     </row>
-    <row r="252" spans="1:5" ht="12.75" hidden="1">
+    <row r="252" spans="1:5" ht="12.75">
       <c r="A252" s="10"/>
       <c r="B252" s="10"/>
       <c r="E252" s="11"/>
     </row>
-    <row r="253" spans="1:5" ht="12.75" hidden="1">
+    <row r="253" spans="1:5" ht="12.75">
       <c r="A253" s="10"/>
       <c r="B253" s="10"/>
       <c r="E253" s="11"/>
     </row>
-    <row r="254" spans="1:5" ht="12.75" hidden="1">
+    <row r="254" spans="1:5" ht="12.75">
       <c r="A254" s="10"/>
       <c r="B254" s="10"/>
       <c r="E254" s="11"/>
     </row>
-    <row r="255" spans="1:5" ht="12.75" hidden="1">
+    <row r="255" spans="1:5" ht="12.75">
       <c r="A255" s="10"/>
       <c r="B255" s="10"/>
       <c r="E255" s="11"/>
     </row>
-    <row r="256" spans="1:5" ht="12.75" hidden="1">
+    <row r="256" spans="1:5" ht="12.75">
       <c r="A256" s="10"/>
       <c r="B256" s="10"/>
       <c r="E256" s="11"/>
     </row>
-    <row r="257" spans="1:5" ht="12.75" hidden="1">
+    <row r="257" spans="1:5" ht="12.75">
       <c r="A257" s="10"/>
       <c r="B257" s="10"/>
       <c r="E257" s="11"/>
     </row>
-    <row r="258" spans="1:5" ht="12.75" hidden="1">
+    <row r="258" spans="1:5" ht="12.75">
       <c r="A258" s="10"/>
       <c r="B258" s="10"/>
       <c r="E258" s="11"/>
     </row>
-    <row r="259" spans="1:5" ht="12.75" hidden="1">
+    <row r="259" spans="1:5" ht="12.75">
       <c r="A259" s="10"/>
       <c r="B259" s="10"/>
       <c r="E259" s="11"/>
     </row>
-    <row r="260" spans="1:5" ht="12.75" hidden="1">
+    <row r="260" spans="1:5" ht="12.75">
       <c r="A260" s="10"/>
       <c r="B260" s="10"/>
       <c r="E260" s="11"/>
     </row>
-    <row r="261" spans="1:5" ht="12.75" hidden="1">
+    <row r="261" spans="1:5" ht="12.75">
       <c r="A261" s="10"/>
       <c r="B261" s="10"/>
       <c r="E261" s="11"/>
     </row>
-    <row r="262" spans="1:5" ht="12.75" hidden="1">
+    <row r="262" spans="1:5" ht="12.75">
       <c r="A262" s="10"/>
       <c r="B262" s="10"/>
       <c r="E262" s="11"/>
     </row>
-    <row r="263" spans="1:5" ht="12.75" hidden="1">
+    <row r="263" spans="1:5" ht="12.75">
       <c r="A263" s="10"/>
       <c r="B263" s="10"/>
       <c r="E263" s="11"/>
     </row>
-    <row r="264" spans="1:5" ht="12.75" hidden="1">
+    <row r="264" spans="1:5" ht="12.75">
       <c r="A264" s="10"/>
       <c r="B264" s="10"/>
       <c r="E264" s="11"/>
     </row>
-    <row r="265" spans="1:5" ht="12.75" hidden="1">
+    <row r="265" spans="1:5" ht="12.75">
       <c r="A265" s="10"/>
       <c r="B265" s="10"/>
       <c r="E265" s="11"/>
     </row>
-    <row r="266" spans="1:5" ht="12.75" hidden="1">
+    <row r="266" spans="1:5" ht="12.75">
       <c r="A266" s="10"/>
       <c r="B266" s="10"/>
       <c r="E266" s="11"/>
     </row>
-    <row r="267" spans="1:5" ht="12.75" hidden="1">
+    <row r="267" spans="1:5" ht="12.75">
       <c r="A267" s="10"/>
       <c r="B267" s="10"/>
       <c r="E267" s="11"/>
     </row>
-    <row r="268" spans="1:5" ht="12.75" hidden="1">
+    <row r="268" spans="1:5" ht="12.75">
       <c r="A268" s="10"/>
       <c r="B268" s="10"/>
       <c r="E268" s="11"/>
     </row>
-    <row r="269" spans="1:5" ht="12.75" hidden="1">
+    <row r="269" spans="1:5" ht="12.75">
       <c r="A269" s="10"/>
       <c r="B269" s="10"/>
       <c r="E269" s="11"/>
     </row>
-    <row r="270" spans="1:5" ht="12.75" hidden="1">
+    <row r="270" spans="1:5" ht="12.75">
       <c r="A270" s="10"/>
       <c r="B270" s="10"/>
       <c r="E270" s="11"/>
     </row>
-    <row r="271" spans="1:5" ht="12.75" hidden="1">
+    <row r="271" spans="1:5" ht="12.75">
       <c r="A271" s="10"/>
       <c r="B271" s="10"/>
       <c r="E271" s="11"/>
     </row>
-    <row r="272" spans="1:5" ht="12.75" hidden="1">
+    <row r="272" spans="1:5" ht="12.75">
       <c r="A272" s="10"/>
       <c r="B272" s="10"/>
       <c r="E272" s="11"/>
     </row>
-    <row r="273" spans="1:5" ht="12.75" hidden="1">
+    <row r="273" spans="1:5" ht="12.75">
       <c r="A273" s="10"/>
       <c r="B273" s="10"/>
       <c r="E273" s="11"/>
     </row>
-    <row r="274" spans="1:5" ht="12.75" hidden="1">
+    <row r="274" spans="1:5" ht="12.75">
       <c r="A274" s="10"/>
       <c r="B274" s="10"/>
       <c r="E274" s="11"/>
     </row>
-    <row r="275" spans="1:5" ht="12.75" hidden="1">
+    <row r="275" spans="1:5" ht="12.75">
       <c r="A275" s="10"/>
       <c r="B275" s="10"/>
       <c r="E275" s="11"/>
     </row>
-    <row r="276" spans="1:5" ht="12.75" hidden="1">
+    <row r="276" spans="1:5" ht="12.75">
       <c r="A276" s="10"/>
       <c r="B276" s="10"/>
       <c r="E276" s="11"/>
     </row>
-    <row r="277" spans="1:5" ht="12.75" hidden="1">
+    <row r="277" spans="1:5" ht="12.75">
       <c r="A277" s="10"/>
       <c r="B277" s="10"/>
       <c r="E277" s="11"/>
     </row>
-    <row r="278" spans="1:5" ht="12.75" hidden="1">
+    <row r="278" spans="1:5" ht="12.75">
       <c r="A278" s="10"/>
       <c r="B278" s="10"/>
       <c r="E278" s="11"/>
     </row>
-    <row r="279" spans="1:5" ht="12.75" hidden="1">
+    <row r="279" spans="1:5" ht="12.75">
       <c r="A279" s="10"/>
       <c r="B279" s="10"/>
       <c r="E279" s="11"/>
     </row>
-    <row r="280" spans="1:5" ht="12.75" hidden="1">
+    <row r="280" spans="1:5" ht="12.75">
       <c r="A280" s="10"/>
       <c r="B280" s="10"/>
       <c r="E280" s="11"/>
     </row>
-    <row r="281" spans="1:5" ht="12.75" hidden="1">
+    <row r="281" spans="1:5" ht="12.75">
       <c r="A281" s="10"/>
       <c r="B281" s="10"/>
       <c r="E281" s="11"/>
     </row>
-    <row r="282" spans="1:5" ht="12.75" hidden="1">
+    <row r="282" spans="1:5" ht="12.75">
       <c r="A282" s="10"/>
       <c r="B282" s="10"/>
       <c r="E282" s="11"/>
     </row>
-    <row r="283" spans="1:5" ht="12.75" hidden="1">
+    <row r="283" spans="1:5" ht="12.75">
       <c r="A283" s="10"/>
       <c r="B283" s="10"/>
       <c r="E283" s="11"/>
     </row>
-    <row r="284" spans="1:5" ht="12.75" hidden="1">
+    <row r="284" spans="1:5" ht="12.75">
       <c r="A284" s="10"/>
       <c r="B284" s="10"/>
       <c r="E284" s="11"/>
     </row>
-    <row r="285" spans="1:5" ht="12.75" hidden="1">
+    <row r="285" spans="1:5" ht="12.75">
       <c r="A285" s="10"/>
       <c r="B285" s="10"/>
       <c r="E285" s="11"/>
     </row>
-    <row r="286" spans="1:5" ht="12.75" hidden="1">
+    <row r="286" spans="1:5" ht="12.75">
       <c r="A286" s="10"/>
       <c r="B286" s="10"/>
       <c r="E286" s="11"/>
     </row>
-    <row r="287" spans="1:5" ht="12.75" hidden="1">
+    <row r="287" spans="1:5" ht="12.75">
       <c r="A287" s="10"/>
       <c r="B287" s="10"/>
       <c r="E287" s="11"/>
     </row>
-    <row r="288" spans="1:5" ht="12.75" hidden="1">
+    <row r="288" spans="1:5" ht="12.75">
       <c r="A288" s="10"/>
       <c r="B288" s="10"/>
       <c r="E288" s="11"/>
     </row>
-    <row r="289" spans="1:5" ht="12.75" hidden="1">
+    <row r="289" spans="1:5" ht="12.75">
       <c r="A289" s="10"/>
       <c r="B289" s="10"/>
       <c r="E289" s="11"/>
     </row>
-    <row r="290" spans="1:5" ht="12.75" hidden="1">
+    <row r="290" spans="1:5" ht="12.75">
       <c r="A290" s="10"/>
       <c r="B290" s="10"/>
       <c r="E290" s="11"/>
     </row>
-    <row r="291" spans="1:5" ht="12.75" hidden="1">
+    <row r="291" spans="1:5" ht="12.75">
       <c r="A291" s="10"/>
       <c r="B291" s="10"/>
       <c r="E291" s="11"/>
     </row>
-    <row r="292" spans="1:5" ht="12.75" hidden="1">
+    <row r="292" spans="1:5" ht="12.75">
       <c r="A292" s="10"/>
       <c r="B292" s="10"/>
       <c r="E292" s="11"/>
     </row>
-    <row r="293" spans="1:5" ht="12.75" hidden="1">
+    <row r="293" spans="1:5" ht="12.75">
       <c r="A293" s="10"/>
       <c r="B293" s="10"/>
       <c r="E293" s="11"/>
     </row>
-    <row r="294" spans="1:5" ht="12.75" hidden="1">
+    <row r="294" spans="1:5" ht="12.75">
       <c r="A294" s="10"/>
       <c r="B294" s="10"/>
       <c r="E294" s="11"/>
     </row>
-    <row r="295" spans="1:5" ht="12.75" hidden="1">
+    <row r="295" spans="1:5" ht="12.75">
       <c r="A295" s="10"/>
       <c r="B295" s="10"/>
       <c r="E295" s="11"/>
     </row>
-    <row r="296" spans="1:5" ht="12.75" hidden="1">
+    <row r="296" spans="1:5" ht="12.75">
       <c r="A296" s="10"/>
       <c r="B296" s="10"/>
       <c r="E296" s="11"/>
     </row>
-    <row r="297" spans="1:5" ht="12.75" hidden="1">
+    <row r="297" spans="1:5" ht="12.75">
       <c r="A297" s="10"/>
       <c r="B297" s="10"/>
       <c r="E297" s="11"/>
     </row>
-    <row r="298" spans="1:5" ht="12.75" hidden="1">
+    <row r="298" spans="1:5" ht="12.75">
       <c r="A298" s="10"/>
       <c r="B298" s="10"/>
       <c r="E298" s="11"/>
     </row>
-    <row r="299" spans="1:5" ht="12.75" hidden="1">
+    <row r="299" spans="1:5" ht="12.75">
       <c r="A299" s="10"/>
       <c r="B299" s="10"/>
       <c r="E299" s="11"/>
     </row>
-    <row r="300" spans="1:5" ht="12.75" hidden="1">
+    <row r="300" spans="1:5" ht="12.75">
       <c r="A300" s="10"/>
       <c r="B300" s="10"/>
       <c r="E300" s="11"/>
     </row>
-    <row r="301" spans="1:5" ht="12.75" hidden="1">
+    <row r="301" spans="1:5" ht="12.75">
       <c r="A301" s="10"/>
       <c r="B301" s="10"/>
       <c r="E301" s="11"/>
     </row>
-    <row r="302" spans="1:5" ht="12.75" hidden="1">
+    <row r="302" spans="1:5" ht="12.75">
       <c r="A302" s="10"/>
       <c r="B302" s="10"/>
       <c r="E302" s="11"/>
     </row>
-    <row r="303" spans="1:5" ht="12.75" hidden="1">
+    <row r="303" spans="1:5" ht="12.75">
       <c r="A303" s="10"/>
       <c r="B303" s="10"/>
       <c r="E303" s="11"/>
     </row>
-    <row r="304" spans="1:5" ht="12.75" hidden="1">
+    <row r="304" spans="1:5" ht="12.75">
       <c r="A304" s="10"/>
       <c r="B304" s="10"/>
       <c r="E304" s="11"/>
     </row>
-    <row r="305" spans="1:5" ht="12.75" hidden="1">
+    <row r="305" spans="1:5" ht="12.75">
       <c r="A305" s="10"/>
       <c r="B305" s="10"/>
       <c r="E305" s="11"/>
     </row>
-    <row r="306" spans="1:5" ht="12.75" hidden="1">
+    <row r="306" spans="1:5" ht="12.75">
       <c r="A306" s="10"/>
       <c r="B306" s="10"/>
       <c r="E306" s="11"/>
     </row>
-    <row r="307" spans="1:5" ht="12.75" hidden="1">
+    <row r="307" spans="1:5" ht="12.75">
       <c r="A307" s="10"/>
       <c r="B307" s="10"/>
       <c r="E307" s="11"/>
     </row>
-    <row r="308" spans="1:5" ht="12.75" hidden="1">
+    <row r="308" spans="1:5" ht="12.75">
       <c r="A308" s="10"/>
       <c r="B308" s="10"/>
       <c r="E308" s="11"/>
     </row>
-    <row r="309" spans="1:5" ht="12.75" hidden="1">
+    <row r="309" spans="1:5" ht="12.75">
       <c r="A309" s="10"/>
       <c r="B309" s="10"/>
       <c r="E309" s="11"/>
     </row>
-    <row r="310" spans="1:5" ht="12.75" hidden="1">
+    <row r="310" spans="1:5" ht="12.75">
       <c r="A310" s="10"/>
       <c r="B310" s="10"/>
       <c r="E310" s="11"/>
     </row>
-    <row r="311" spans="1:5" ht="12.75" hidden="1">
+    <row r="311" spans="1:5" ht="12.75">
       <c r="A311" s="10"/>
       <c r="B311" s="10"/>
       <c r="E311" s="11"/>
     </row>
-    <row r="312" spans="1:5" ht="12.75" hidden="1">
+    <row r="312" spans="1:5" ht="12.75">
       <c r="A312" s="10"/>
       <c r="B312" s="10"/>
       <c r="E312" s="11"/>
     </row>
-    <row r="313" spans="1:5" ht="12.75" hidden="1">
+    <row r="313" spans="1:5" ht="12.75">
       <c r="A313" s="10"/>
       <c r="B313" s="10"/>
       <c r="E313" s="11"/>
     </row>
-    <row r="314" spans="1:5" ht="12.75" hidden="1">
+    <row r="314" spans="1:5" ht="12.75">
       <c r="A314" s="10"/>
       <c r="B314" s="10"/>
       <c r="E314" s="11"/>
     </row>
-    <row r="315" spans="1:5" ht="12.75" hidden="1">
+    <row r="315" spans="1:5" ht="12.75">
       <c r="A315" s="10"/>
       <c r="B315" s="10"/>
       <c r="E315" s="11"/>
     </row>
-    <row r="316" spans="1:5" ht="12.75" hidden="1">
+    <row r="316" spans="1:5" ht="12.75">
       <c r="A316" s="10"/>
       <c r="B316" s="10"/>
       <c r="E316" s="11"/>
     </row>
-    <row r="317" spans="1:5" ht="12.75" hidden="1">
+    <row r="317" spans="1:5" ht="12.75">
       <c r="A317" s="10"/>
       <c r="B317" s="10"/>
       <c r="E317" s="11"/>
     </row>
-    <row r="318" spans="1:5" ht="12.75" hidden="1">
+    <row r="318" spans="1:5" ht="12.75">
       <c r="A318" s="10"/>
       <c r="B318" s="10"/>
       <c r="E318" s="11"/>
     </row>
-    <row r="319" spans="1:5" ht="12.75" hidden="1">
+    <row r="319" spans="1:5" ht="12.75">
       <c r="A319" s="10"/>
       <c r="B319" s="10"/>
       <c r="E319" s="11"/>
     </row>
-    <row r="320" spans="1:5" ht="12.75" hidden="1">
+    <row r="320" spans="1:5" ht="12.75">
       <c r="A320" s="10"/>
       <c r="B320" s="10"/>
       <c r="E320" s="11"/>
     </row>
-    <row r="321" spans="1:5" ht="12.75" hidden="1">
+    <row r="321" spans="1:5" ht="12.75">
       <c r="A321" s="10"/>
       <c r="B321" s="10"/>
       <c r="E321" s="11"/>
     </row>
-    <row r="322" spans="1:5" ht="12.75" hidden="1">
+    <row r="322" spans="1:5" ht="12.75">
       <c r="A322" s="10"/>
       <c r="B322" s="10"/>
       <c r="E322" s="11"/>
     </row>
-    <row r="323" spans="1:5" ht="12.75" hidden="1">
+    <row r="323" spans="1:5" ht="12.75">
       <c r="A323" s="10"/>
       <c r="B323" s="10"/>
       <c r="E323" s="11"/>
     </row>
-    <row r="324" spans="1:5" ht="12.75" hidden="1">
+    <row r="324" spans="1:5" ht="12.75">
       <c r="A324" s="10"/>
       <c r="B324" s="10"/>
       <c r="E324" s="11"/>
     </row>
-    <row r="325" spans="1:5" ht="12.75" hidden="1">
+    <row r="325" spans="1:5" ht="12.75">
       <c r="A325" s="10"/>
       <c r="B325" s="10"/>
       <c r="E325" s="11"/>
     </row>
-    <row r="326" spans="1:5" ht="12.75" hidden="1">
+    <row r="326" spans="1:5" ht="12.75">
       <c r="A326" s="10"/>
       <c r="B326" s="10"/>
       <c r="E326" s="11"/>
     </row>
-    <row r="327" spans="1:5" ht="12.75" hidden="1">
+    <row r="327" spans="1:5" ht="12.75">
       <c r="A327" s="10"/>
       <c r="B327" s="10"/>
       <c r="E327" s="11"/>
     </row>
-    <row r="328" spans="1:5" ht="12.75" hidden="1">
+    <row r="328" spans="1:5" ht="12.75">
       <c r="A328" s="10"/>
       <c r="B328" s="10"/>
       <c r="E328" s="11"/>
     </row>
-    <row r="329" spans="1:5" ht="12.75" hidden="1">
+    <row r="329" spans="1:5" ht="12.75">
       <c r="A329" s="10"/>
       <c r="B329" s="10"/>
       <c r="E329" s="11"/>
     </row>
-    <row r="330" spans="1:5" ht="12.75" hidden="1">
+    <row r="330" spans="1:5" ht="12.75">
       <c r="A330" s="10"/>
       <c r="B330" s="10"/>
       <c r="E330" s="11"/>
     </row>
-    <row r="331" spans="1:5" ht="12.75" hidden="1">
+    <row r="331" spans="1:5" ht="12.75">
       <c r="A331" s="10"/>
       <c r="B331" s="10"/>
       <c r="E331" s="11"/>
     </row>
-    <row r="332" spans="1:5" ht="12.75" hidden="1">
+    <row r="332" spans="1:5" ht="12.75">
       <c r="A332" s="10"/>
       <c r="B332" s="10"/>
       <c r="E332" s="11"/>
     </row>
-    <row r="333" spans="1:5" ht="12.75" hidden="1">
+    <row r="333" spans="1:5" ht="12.75">
       <c r="A333" s="10"/>
       <c r="B333" s="10"/>
       <c r="E333" s="11"/>
     </row>
-    <row r="334" spans="1:5" ht="12.75" hidden="1">
+    <row r="334" spans="1:5" ht="12.75">
       <c r="A334" s="10"/>
       <c r="B334" s="10"/>
       <c r="E334" s="11"/>
     </row>
-    <row r="335" spans="1:5" ht="12.75" hidden="1">
+    <row r="335" spans="1:5" ht="12.75">
       <c r="A335" s="10"/>
       <c r="B335" s="10"/>
       <c r="E335" s="11"/>
     </row>
-    <row r="336" spans="1:5" ht="12.75" hidden="1">
+    <row r="336" spans="1:5" ht="12.75">
       <c r="A336" s="10"/>
       <c r="B336" s="10"/>
       <c r="E336" s="11"/>
     </row>
-    <row r="337" spans="1:5" ht="12.75" hidden="1">
+    <row r="337" spans="1:5" ht="12.75">
       <c r="A337" s="10"/>
       <c r="B337" s="10"/>
       <c r="E337" s="11"/>
     </row>
-    <row r="338" spans="1:5" ht="12.75" hidden="1">
+    <row r="338" spans="1:5" ht="12.75">
       <c r="A338" s="10"/>
       <c r="B338" s="10"/>
       <c r="E338" s="11"/>
     </row>
-    <row r="339" spans="1:5" ht="12.75" hidden="1">
+    <row r="339" spans="1:5" ht="12.75">
       <c r="A339" s="10"/>
       <c r="B339" s="10"/>
       <c r="E339" s="11"/>
     </row>
-    <row r="340" spans="1:5" ht="12.75" hidden="1">
+    <row r="340" spans="1:5" ht="12.75">
       <c r="A340" s="10"/>
       <c r="B340" s="10"/>
       <c r="E340" s="11"/>
     </row>
-    <row r="341" spans="1:5" ht="12.75" hidden="1">
+    <row r="341" spans="1:5" ht="12.75">
       <c r="A341" s="10"/>
       <c r="B341" s="10"/>
       <c r="E341" s="11"/>
     </row>
-    <row r="342" spans="1:5" ht="12.75" hidden="1">
+    <row r="342" spans="1:5" ht="12.75">
       <c r="A342" s="10"/>
       <c r="B342" s="10"/>
       <c r="E342" s="11"/>
     </row>
-    <row r="343" spans="1:5" ht="12.75" hidden="1">
+    <row r="343" spans="1:5" ht="12.75">
       <c r="A343" s="10"/>
       <c r="B343" s="10"/>
       <c r="E343" s="11"/>
     </row>
-    <row r="344" spans="1:5" ht="12.75" hidden="1">
+    <row r="344" spans="1:5" ht="12.75">
       <c r="A344" s="10"/>
       <c r="B344" s="10"/>
       <c r="E344" s="11"/>
     </row>
-    <row r="345" spans="1:5" ht="12.75" hidden="1">
+    <row r="345" spans="1:5" ht="12.75">
       <c r="A345" s="10"/>
       <c r="B345" s="10"/>
       <c r="E345" s="11"/>
     </row>
-    <row r="346" spans="1:5" ht="12.75" hidden="1">
+    <row r="346" spans="1:5" ht="12.75">
       <c r="A346" s="10"/>
       <c r="B346" s="10"/>
       <c r="E346" s="11"/>
     </row>
-    <row r="347" spans="1:5" ht="12.75" hidden="1">
+    <row r="347" spans="1:5" ht="12.75">
       <c r="A347" s="10"/>
       <c r="B347" s="10"/>
       <c r="E347" s="11"/>
     </row>
-    <row r="348" spans="1:5" ht="12.75" hidden="1">
+    <row r="348" spans="1:5" ht="12.75">
       <c r="A348" s="10"/>
       <c r="B348" s="10"/>
       <c r="E348" s="11"/>
     </row>
-    <row r="349" spans="1:5" ht="12.75" hidden="1">
+    <row r="349" spans="1:5" ht="12.75">
       <c r="A349" s="10"/>
       <c r="B349" s="10"/>
       <c r="E349" s="11"/>
     </row>
-    <row r="350" spans="1:5" ht="12.75" hidden="1">
+    <row r="350" spans="1:5" ht="12.75">
       <c r="A350" s="10"/>
       <c r="B350" s="10"/>
       <c r="E350" s="11"/>
     </row>
-    <row r="351" spans="1:5" ht="12.75" hidden="1">
+    <row r="351" spans="1:5" ht="12.75">
       <c r="A351" s="10"/>
       <c r="B351" s="10"/>
       <c r="E351" s="11"/>
     </row>
-    <row r="352" spans="1:5" ht="12.75" hidden="1">
+    <row r="352" spans="1:5" ht="12.75">
       <c r="A352" s="10"/>
       <c r="B352" s="10"/>
       <c r="E352" s="11"/>
     </row>
-    <row r="353" spans="1:5" ht="12.75" hidden="1">
+    <row r="353" spans="1:5" ht="12.75">
       <c r="A353" s="10"/>
       <c r="B353" s="10"/>
       <c r="E353" s="11"/>
     </row>
-    <row r="354" spans="1:5" ht="12.75" hidden="1">
+    <row r="354" spans="1:5" ht="12.75">
       <c r="A354" s="10"/>
       <c r="B354" s="10"/>
       <c r="E354" s="11"/>
     </row>
-    <row r="355" spans="1:5" ht="12.75" hidden="1">
+    <row r="355" spans="1:5" ht="12.75">
       <c r="A355" s="10"/>
       <c r="B355" s="10"/>
       <c r="E355" s="11"/>
     </row>
-    <row r="356" spans="1:5" ht="12.75" hidden="1">
+    <row r="356" spans="1:5" ht="12.75">
       <c r="A356" s="10"/>
       <c r="B356" s="10"/>
       <c r="E356" s="11"/>
     </row>
-    <row r="357" spans="1:5" ht="12.75" hidden="1">
+    <row r="357" spans="1:5" ht="12.75">
       <c r="A357" s="10"/>
       <c r="B357" s="10"/>
       <c r="E357" s="11"/>
     </row>
-    <row r="358" spans="1:5" ht="12.75" hidden="1">
+    <row r="358" spans="1:5" ht="12.75">
       <c r="A358" s="10"/>
       <c r="B358" s="10"/>
       <c r="E358" s="11"/>
     </row>
-    <row r="359" spans="1:5" ht="12.75" hidden="1">
+    <row r="359" spans="1:5" ht="12.75">
       <c r="A359" s="10"/>
       <c r="B359" s="10"/>
       <c r="E359" s="11"/>
     </row>
-    <row r="360" spans="1:5" ht="12.75" hidden="1">
+    <row r="360" spans="1:5" ht="12.75">
       <c r="A360" s="10"/>
       <c r="B360" s="10"/>
       <c r="E360" s="11"/>
     </row>
-    <row r="361" spans="1:5" ht="12.75" hidden="1">
+    <row r="361" spans="1:5" ht="12.75">
       <c r="A361" s="10"/>
       <c r="B361" s="10"/>
       <c r="E361" s="11"/>
     </row>
-    <row r="362" spans="1:5" ht="12.75" hidden="1">
+    <row r="362" spans="1:5" ht="12.75">
       <c r="A362" s="10"/>
       <c r="B362" s="10"/>
       <c r="E362" s="11"/>
     </row>
-    <row r="363" spans="1:5" ht="12.75" hidden="1">
+    <row r="363" spans="1:5" ht="12.75">
       <c r="A363" s="10"/>
       <c r="B363" s="10"/>
       <c r="E363" s="11"/>
     </row>
-    <row r="364" spans="1:5" ht="12.75" hidden="1">
+    <row r="364" spans="1:5" ht="12.75">
       <c r="A364" s="10"/>
       <c r="B364" s="10"/>
       <c r="E364" s="11"/>
     </row>
-    <row r="365" spans="1:5" ht="12.75" hidden="1">
+    <row r="365" spans="1:5" ht="12.75">
       <c r="A365" s="10"/>
       <c r="B365" s="10"/>
       <c r="E365" s="11"/>
     </row>
-    <row r="366" spans="1:5" ht="12.75" hidden="1">
+    <row r="366" spans="1:5" ht="12.75">
       <c r="A366" s="10"/>
       <c r="B366" s="10"/>
       <c r="E366" s="11"/>
     </row>
-    <row r="367" spans="1:5" ht="12.75" hidden="1">
+    <row r="367" spans="1:5" ht="12.75">
       <c r="A367" s="10"/>
       <c r="B367" s="10"/>
       <c r="E367" s="11"/>
     </row>
-    <row r="368" spans="1:5" ht="12.75" hidden="1">
+    <row r="368" spans="1:5" ht="12.75">
       <c r="A368" s="10"/>
       <c r="B368" s="10"/>
       <c r="E368" s="11"/>
     </row>
-    <row r="369" spans="1:5" ht="12.75" hidden="1">
+    <row r="369" spans="1:5" ht="12.75">
       <c r="A369" s="10"/>
       <c r="B369" s="10"/>
       <c r="E369" s="11"/>
     </row>
-    <row r="370" spans="1:5" ht="12.75" hidden="1">
+    <row r="370" spans="1:5" ht="12.75">
       <c r="A370" s="10"/>
       <c r="B370" s="10"/>
       <c r="E370" s="11"/>
     </row>
-    <row r="371" spans="1:5" ht="12.75" hidden="1">
+    <row r="371" spans="1:5" ht="12.75">
       <c r="A371" s="10"/>
       <c r="B371" s="10"/>
       <c r="E371" s="11"/>
     </row>
-    <row r="372" spans="1:5" ht="12.75" hidden="1">
+    <row r="372" spans="1:5" ht="12.75">
       <c r="A372" s="10"/>
       <c r="B372" s="10"/>
       <c r="E372" s="11"/>
     </row>
-    <row r="373" spans="1:5" ht="12.75" hidden="1">
+    <row r="373" spans="1:5" ht="12.75">
       <c r="A373" s="10"/>
       <c r="B373" s="10"/>
       <c r="E373" s="11"/>
     </row>
-    <row r="374" spans="1:5" ht="12.75" hidden="1">
+    <row r="374" spans="1:5" ht="12.75">
       <c r="A374" s="10"/>
       <c r="B374" s="10"/>
       <c r="E374" s="11"/>
     </row>
-    <row r="375" spans="1:5" ht="12.75" hidden="1">
+    <row r="375" spans="1:5" ht="12.75">
       <c r="A375" s="10"/>
       <c r="B375" s="10"/>
       <c r="E375" s="11"/>
     </row>
-    <row r="376" spans="1:5" ht="12.75" hidden="1">
+    <row r="376" spans="1:5" ht="12.75">
       <c r="A376" s="10"/>
       <c r="B376" s="10"/>
       <c r="E376" s="11"/>
     </row>
-    <row r="377" spans="1:5" ht="12.75" hidden="1">
+    <row r="377" spans="1:5" ht="12.75">
       <c r="A377" s="10"/>
       <c r="B377" s="10"/>
       <c r="E377" s="11"/>
     </row>
-    <row r="378" spans="1:5" ht="12.75" hidden="1">
+    <row r="378" spans="1:5" ht="12.75">
       <c r="A378" s="10"/>
       <c r="B378" s="10"/>
       <c r="E378" s="11"/>
     </row>
-    <row r="379" spans="1:5" ht="12.75" hidden="1">
+    <row r="379" spans="1:5" ht="12.75">
       <c r="A379" s="10"/>
       <c r="B379" s="10"/>
       <c r="E379" s="11"/>
     </row>
-    <row r="380" spans="1:5" ht="12.75" hidden="1">
+    <row r="380" spans="1:5" ht="12.75">
       <c r="A380" s="10"/>
       <c r="B380" s="10"/>
       <c r="E380" s="11"/>
     </row>
-    <row r="381" spans="1:5" ht="12.75" hidden="1">
+    <row r="381" spans="1:5" ht="12.75">
       <c r="A381" s="10"/>
       <c r="B381" s="10"/>
       <c r="E381" s="11"/>
     </row>
-    <row r="382" spans="1:5" ht="12.75" hidden="1">
+    <row r="382" spans="1:5" ht="12.75">
       <c r="A382" s="10"/>
       <c r="B382" s="10"/>
       <c r="E382" s="11"/>
     </row>
-    <row r="383" spans="1:5" ht="12.75" hidden="1">
+    <row r="383" spans="1:5" ht="12.75">
       <c r="A383" s="10"/>
       <c r="B383" s="10"/>
       <c r="E383" s="11"/>
     </row>
-    <row r="384" spans="1:5" ht="12.75" hidden="1">
+    <row r="384" spans="1:5" ht="12.75">
       <c r="A384" s="10"/>
       <c r="B384" s="10"/>
       <c r="E384" s="11"/>
     </row>
-    <row r="385" spans="1:5" ht="12.75" hidden="1">
+    <row r="385" spans="1:5" ht="12.75">
       <c r="A385" s="10"/>
       <c r="B385" s="10"/>
       <c r="E385" s="11"/>
     </row>
-    <row r="386" spans="1:5" ht="12.75" hidden="1">
+    <row r="386" spans="1:5" ht="12.75">
       <c r="A386" s="10"/>
       <c r="B386" s="10"/>
       <c r="E386" s="11"/>
     </row>
-    <row r="387" spans="1:5" ht="12.75" hidden="1">
+    <row r="387" spans="1:5" ht="12.75">
       <c r="A387" s="10"/>
       <c r="B387" s="10"/>
       <c r="E387" s="11"/>
     </row>
-    <row r="388" spans="1:5" ht="12.75" hidden="1">
+    <row r="388" spans="1:5" ht="12.75">
       <c r="A388" s="10"/>
       <c r="B388" s="10"/>
       <c r="E388" s="11"/>
     </row>
-    <row r="389" spans="1:5" ht="12.75" hidden="1">
+    <row r="389" spans="1:5" ht="12.75">
       <c r="A389" s="10"/>
       <c r="B389" s="10"/>
       <c r="E389" s="11"/>
     </row>
-    <row r="390" spans="1:5" ht="12.75" hidden="1">
+    <row r="390" spans="1:5" ht="12.75">
       <c r="A390" s="10"/>
       <c r="B390" s="10"/>
       <c r="E390" s="11"/>
     </row>
-    <row r="391" spans="1:5" ht="12.75" hidden="1">
+    <row r="391" spans="1:5" ht="12.75">
       <c r="A391" s="10"/>
       <c r="B391" s="10"/>
       <c r="E391" s="11"/>
     </row>
-    <row r="392" spans="1:5" ht="12.75" hidden="1">
+    <row r="392" spans="1:5" ht="12.75">
       <c r="A392" s="10"/>
       <c r="B392" s="10"/>
       <c r="E392" s="11"/>
     </row>
-    <row r="393" spans="1:5" ht="12.75" hidden="1">
+    <row r="393" spans="1:5" ht="12.75">
       <c r="A393" s="10"/>
       <c r="B393" s="10"/>
       <c r="E393" s="11"/>
     </row>
-    <row r="394" spans="1:5" ht="12.75" hidden="1">
+    <row r="394" spans="1:5" ht="12.75">
       <c r="A394" s="10"/>
       <c r="B394" s="10"/>
       <c r="E394" s="11"/>
     </row>
-    <row r="395" spans="1:5" ht="12.75" hidden="1">
+    <row r="395" spans="1:5" ht="12.75">
       <c r="A395" s="10"/>
       <c r="B395" s="10"/>
       <c r="E395" s="11"/>
     </row>
-    <row r="396" spans="1:5" ht="12.75" hidden="1">
+    <row r="396" spans="1:5" ht="12.75">
       <c r="A396" s="10"/>
       <c r="B396" s="10"/>
       <c r="E396" s="11"/>
     </row>
-    <row r="397" spans="1:5" ht="12.75" hidden="1">
+    <row r="397" spans="1:5" ht="12.75">
       <c r="A397" s="10"/>
       <c r="B397" s="10"/>
       <c r="E397" s="11"/>
     </row>
-    <row r="398" spans="1:5" ht="12.75" hidden="1">
+    <row r="398" spans="1:5" ht="12.75">
       <c r="A398" s="10"/>
       <c r="B398" s="10"/>
       <c r="E398" s="11"/>
     </row>
-    <row r="399" spans="1:5" ht="12.75" hidden="1">
+    <row r="399" spans="1:5" ht="12.75">
       <c r="A399" s="10"/>
       <c r="B399" s="10"/>
       <c r="E399" s="11"/>
     </row>
-    <row r="400" spans="1:5" ht="12.75" hidden="1">
+    <row r="400" spans="1:5" ht="12.75">
       <c r="A400" s="10"/>
       <c r="B400" s="10"/>
       <c r="E400" s="11"/>
     </row>
-    <row r="401" spans="1:5" ht="12.75" hidden="1">
+    <row r="401" spans="1:5" ht="12.75">
       <c r="A401" s="10"/>
       <c r="B401" s="10"/>
       <c r="E401" s="11"/>
     </row>
-    <row r="402" spans="1:5" ht="12.75" hidden="1">
+    <row r="402" spans="1:5" ht="12.75">
       <c r="A402" s="10"/>
       <c r="B402" s="10"/>
       <c r="E402" s="11"/>
     </row>
-    <row r="403" spans="1:5" ht="12.75" hidden="1">
+    <row r="403" spans="1:5" ht="12.75">
       <c r="A403" s="10"/>
       <c r="B403" s="10"/>
       <c r="E403" s="11"/>
     </row>
-    <row r="404" spans="1:5" ht="12.75" hidden="1">
+    <row r="404" spans="1:5" ht="12.75">
       <c r="A404" s="10"/>
       <c r="B404" s="10"/>
       <c r="E404" s="11"/>
     </row>
-    <row r="405" spans="1:5" ht="12.75" hidden="1">
+    <row r="405" spans="1:5" ht="12.75">
       <c r="A405" s="10"/>
       <c r="B405" s="10"/>
       <c r="E405" s="11"/>
     </row>
-    <row r="406" spans="1:5" ht="12.75" hidden="1">
+    <row r="406" spans="1:5" ht="12.75">
       <c r="A406" s="10"/>
       <c r="B406" s="10"/>
       <c r="E406" s="11"/>
     </row>
-    <row r="407" spans="1:5" ht="12.75" hidden="1">
+    <row r="407" spans="1:5" ht="12.75">
       <c r="A407" s="10"/>
       <c r="B407" s="10"/>
       <c r="E407" s="11"/>
     </row>
-    <row r="408" spans="1:5" ht="12.75" hidden="1">
+    <row r="408" spans="1:5" ht="12.75">
       <c r="A408" s="10"/>
       <c r="B408" s="10"/>
       <c r="E408" s="11"/>
     </row>
-    <row r="409" spans="1:5" ht="12.75" hidden="1">
+    <row r="409" spans="1:5" ht="12.75">
       <c r="A409" s="10"/>
       <c r="B409" s="10"/>
       <c r="E409" s="11"/>
     </row>
-    <row r="410" spans="1:5" ht="12.75" hidden="1">
+    <row r="410" spans="1:5" ht="12.75">
       <c r="A410" s="10"/>
       <c r="B410" s="10"/>
       <c r="E410" s="11"/>
     </row>
-    <row r="411" spans="1:5" ht="12.75" hidden="1">
+    <row r="411" spans="1:5" ht="12.75">
       <c r="A411" s="10"/>
       <c r="B411" s="10"/>
       <c r="E411" s="11"/>
     </row>
-    <row r="412" spans="1:5" ht="12.75" hidden="1">
+    <row r="412" spans="1:5" ht="12.75">
       <c r="A412" s="10"/>
       <c r="B412" s="10"/>
       <c r="E412" s="11"/>
     </row>
-    <row r="413" spans="1:5" ht="12.75" hidden="1">
+    <row r="413" spans="1:5" ht="12.75">
       <c r="A413" s="10"/>
       <c r="B413" s="10"/>
       <c r="E413" s="11"/>
     </row>
-    <row r="414" spans="1:5" ht="12.75" hidden="1">
+    <row r="414" spans="1:5" ht="12.75">
       <c r="A414" s="10"/>
       <c r="B414" s="10"/>
       <c r="E414" s="11"/>
     </row>
-    <row r="415" spans="1:5" ht="12.75" hidden="1">
+    <row r="415" spans="1:5" ht="12.75">
       <c r="A415" s="10"/>
       <c r="B415" s="10"/>
       <c r="E415" s="11"/>
     </row>
-    <row r="416" spans="1:5" ht="12.75" hidden="1">
+    <row r="416" spans="1:5" ht="12.75">
       <c r="A416" s="10"/>
       <c r="B416" s="10"/>
       <c r="E416" s="11"/>
     </row>
-    <row r="417" spans="1:5" ht="12.75" hidden="1">
+    <row r="417" spans="1:5" ht="12.75">
       <c r="A417" s="10"/>
       <c r="B417" s="10"/>
       <c r="E417" s="11"/>
     </row>
-    <row r="418" spans="1:5" ht="12.75" hidden="1">
+    <row r="418" spans="1:5" ht="12.75">
       <c r="A418" s="10"/>
       <c r="B418" s="10"/>
       <c r="E418" s="11"/>
     </row>
-    <row r="419" spans="1:5" ht="12.75" hidden="1">
+    <row r="419" spans="1:5" ht="12.75">
       <c r="A419" s="10"/>
       <c r="B419" s="10"/>
       <c r="E419" s="11"/>
     </row>
-    <row r="420" spans="1:5" ht="12.75" hidden="1">
+    <row r="420" spans="1:5" ht="12.75">
       <c r="A420" s="10"/>
       <c r="B420" s="10"/>
       <c r="E420" s="11"/>
     </row>
-    <row r="421" spans="1:5" ht="12.75" hidden="1">
+    <row r="421" spans="1:5" ht="12.75">
       <c r="A421" s="10"/>
       <c r="B421" s="10"/>
       <c r="E421" s="11"/>
     </row>
-    <row r="422" spans="1:5" ht="12.75" hidden="1">
+    <row r="422" spans="1:5" ht="12.75">
       <c r="A422" s="10"/>
       <c r="B422" s="10"/>
       <c r="E422" s="11"/>
     </row>
-    <row r="423" spans="1:5" ht="12.75" hidden="1">
+    <row r="423" spans="1:5" ht="12.75">
       <c r="A423" s="10"/>
       <c r="B423" s="10"/>
       <c r="E423" s="11"/>
     </row>
-    <row r="424" spans="1:5" ht="12.75" hidden="1">
+    <row r="424" spans="1:5" ht="12.75">
       <c r="A424" s="10"/>
       <c r="B424" s="10"/>
       <c r="E424" s="11"/>
     </row>
-    <row r="425" spans="1:5" ht="12.75" hidden="1">
+    <row r="425" spans="1:5" ht="12.75">
       <c r="A425" s="10"/>
       <c r="B425" s="10"/>
       <c r="E425" s="11"/>
     </row>
-    <row r="426" spans="1:5" ht="12.75" hidden="1">
+    <row r="426" spans="1:5" ht="12.75">
       <c r="A426" s="10"/>
       <c r="B426" s="10"/>
       <c r="E426" s="11"/>
     </row>
-    <row r="427" spans="1:5" ht="12.75" hidden="1">
+    <row r="427" spans="1:5" ht="12.75">
       <c r="A427" s="10"/>
       <c r="B427" s="10"/>
       <c r="E427" s="11"/>
     </row>
-    <row r="428" spans="1:5" ht="12.75" hidden="1">
+    <row r="428" spans="1:5" ht="12.75">
       <c r="A428" s="10"/>
       <c r="B428" s="10"/>
       <c r="E428" s="11"/>
     </row>
-    <row r="429" spans="1:5" ht="12.75" hidden="1">
+    <row r="429" spans="1:5" ht="12.75">
       <c r="A429" s="10"/>
       <c r="B429" s="10"/>
       <c r="E429" s="11"/>
     </row>
-    <row r="430" spans="1:5" ht="12.75" hidden="1">
+    <row r="430" spans="1:5" ht="12.75">
       <c r="A430" s="10"/>
       <c r="B430" s="10"/>
       <c r="E430" s="11"/>
     </row>
-    <row r="431" spans="1:5" ht="12.75" hidden="1">
+    <row r="431" spans="1:5" ht="12.75">
       <c r="A431" s="10"/>
       <c r="B431" s="10"/>
       <c r="E431" s="11"/>
     </row>
-    <row r="432" spans="1:5" ht="12.75" hidden="1">
+    <row r="432" spans="1:5" ht="12.75">
       <c r="A432" s="10"/>
       <c r="B432" s="10"/>
       <c r="E432" s="11"/>
     </row>
-    <row r="433" spans="1:5" ht="12.75" hidden="1">
+    <row r="433" spans="1:5" ht="12.75">
       <c r="A433" s="10"/>
       <c r="B433" s="10"/>
       <c r="E433" s="11"/>
     </row>
-    <row r="434" spans="1:5" ht="12.75" hidden="1">
+    <row r="434" spans="1:5" ht="12.75">
       <c r="A434" s="10"/>
       <c r="B434" s="10"/>
       <c r="E434" s="11"/>
     </row>
-    <row r="435" spans="1:5" ht="12.75" hidden="1">
+    <row r="435" spans="1:5" ht="12.75">
       <c r="A435" s="10"/>
       <c r="B435" s="10"/>
       <c r="E435" s="11"/>
     </row>
-    <row r="436" spans="1:5" ht="12.75" hidden="1">
+    <row r="436" spans="1:5" ht="12.75">
       <c r="A436" s="10"/>
       <c r="B436" s="10"/>
       <c r="E436" s="11"/>
     </row>
-    <row r="437" spans="1:5" ht="12.75" hidden="1">
+    <row r="437" spans="1:5" ht="12.75">
       <c r="A437" s="10"/>
       <c r="B437" s="10"/>
       <c r="E437" s="11"/>
     </row>
-    <row r="438" spans="1:5" ht="12.75" hidden="1">
+    <row r="438" spans="1:5" ht="12.75">
       <c r="A438" s="10"/>
       <c r="B438" s="10"/>
       <c r="E438" s="11"/>
     </row>
-    <row r="439" spans="1:5" ht="12.75" hidden="1">
+    <row r="439" spans="1:5" ht="12.75">
       <c r="A439" s="10"/>
       <c r="B439" s="10"/>
       <c r="E439" s="11"/>
     </row>
-    <row r="440" spans="1:5" ht="12.75" hidden="1">
+    <row r="440" spans="1:5" ht="12.75">
       <c r="A440" s="10"/>
       <c r="B440" s="10"/>
       <c r="E440" s="11"/>
     </row>
-    <row r="441" spans="1:5" ht="12.75" hidden="1">
+    <row r="441" spans="1:5" ht="12.75">
       <c r="A441" s="10"/>
       <c r="B441" s="10"/>
       <c r="E441" s="11"/>
     </row>
-    <row r="442" spans="1:5" ht="12.75" hidden="1">
+    <row r="442" spans="1:5" ht="12.75">
       <c r="A442" s="10"/>
       <c r="B442" s="10"/>
       <c r="E442" s="11"/>
     </row>
-    <row r="443" spans="1:5" ht="12.75" hidden="1">
+    <row r="443" spans="1:5" ht="12.75">
       <c r="A443" s="10"/>
       <c r="B443" s="10"/>
       <c r="E443" s="11"/>
     </row>
-    <row r="444" spans="1:5" ht="12.75" hidden="1">
+    <row r="444" spans="1:5" ht="12.75">
       <c r="A444" s="10"/>
       <c r="B444" s="10"/>
       <c r="E444" s="11"/>
     </row>
-    <row r="445" spans="1:5" ht="12.75" hidden="1">
+    <row r="445" spans="1:5" ht="12.75">
       <c r="A445" s="10"/>
       <c r="B445" s="10"/>
       <c r="E445" s="11"/>
     </row>
-    <row r="446" spans="1:5" ht="12.75" hidden="1">
+    <row r="446" spans="1:5" ht="12.75">
       <c r="A446" s="10"/>
       <c r="B446" s="10"/>
       <c r="E446" s="11"/>
     </row>
-    <row r="447" spans="1:5" ht="12.75" hidden="1">
+    <row r="447" spans="1:5" ht="12.75">
       <c r="A447" s="10"/>
       <c r="B447" s="10"/>
       <c r="E447" s="11"/>
     </row>
-    <row r="448" spans="1:5" ht="12.75" hidden="1">
+    <row r="448" spans="1:5" ht="12.75">
       <c r="A448" s="10"/>
       <c r="B448" s="10"/>
       <c r="E448" s="11"/>
     </row>
-    <row r="449" spans="1:5" ht="12.75" hidden="1">
+    <row r="449" spans="1:5" ht="12.75">
       <c r="A449" s="10"/>
       <c r="B449" s="10"/>
       <c r="E449" s="11"/>
     </row>
-    <row r="450" spans="1:5" ht="12.75" hidden="1">
+    <row r="450" spans="1:5" ht="12.75">
       <c r="A450" s="10"/>
       <c r="B450" s="10"/>
       <c r="E450" s="11"/>
     </row>
-    <row r="451" spans="1:5" ht="12.75" hidden="1">
+    <row r="451" spans="1:5" ht="12.75">
       <c r="A451" s="10"/>
       <c r="B451" s="10"/>
       <c r="E451" s="11"/>
     </row>
-    <row r="452" spans="1:5" ht="12.75" hidden="1">
+    <row r="452" spans="1:5" ht="12.75">
       <c r="A452" s="10"/>
       <c r="B452" s="10"/>
       <c r="E452" s="11"/>
     </row>
-    <row r="453" spans="1:5" ht="12.75" hidden="1">
+    <row r="453" spans="1:5" ht="12.75">
       <c r="A453" s="10"/>
       <c r="B453" s="10"/>
       <c r="E453" s="11"/>
     </row>
-    <row r="454" spans="1:5" ht="12.75" hidden="1">
+    <row r="454" spans="1:5" ht="12.75">
       <c r="A454" s="10"/>
       <c r="B454" s="10"/>
       <c r="E454" s="11"/>
     </row>
-    <row r="455" spans="1:5" ht="12.75" hidden="1">
+    <row r="455" spans="1:5" ht="12.75">
       <c r="A455" s="10"/>
       <c r="B455" s="10"/>
       <c r="E455" s="11"/>
     </row>
-    <row r="456" spans="1:5" ht="12.75" hidden="1">
+    <row r="456" spans="1:5" ht="12.75">
       <c r="A456" s="10"/>
       <c r="B456" s="10"/>
       <c r="E456" s="11"/>
     </row>
-    <row r="457" spans="1:5" ht="12.75" hidden="1">
+    <row r="457" spans="1:5" ht="12.75">
       <c r="A457" s="10"/>
       <c r="B457" s="10"/>
       <c r="E457" s="11"/>
     </row>
-    <row r="458" spans="1:5" ht="12.75" hidden="1">
+    <row r="458" spans="1:5" ht="12.75">
       <c r="A458" s="10"/>
       <c r="B458" s="10"/>
       <c r="E458" s="11"/>
     </row>
-    <row r="459" spans="1:5" ht="12.75" hidden="1">
+    <row r="459" spans="1:5" ht="12.75">
       <c r="A459" s="10"/>
       <c r="B459" s="10"/>
       <c r="E459" s="11"/>
     </row>
-    <row r="460" spans="1:5" ht="12.75" hidden="1">
+    <row r="460" spans="1:5" ht="12.75">
       <c r="A460" s="10"/>
       <c r="B460" s="10"/>
       <c r="E460" s="11"/>
     </row>
-    <row r="461" spans="1:5" ht="12.75" hidden="1">
+    <row r="461" spans="1:5" ht="12.75">
       <c r="A461" s="10"/>
       <c r="B461" s="10"/>
       <c r="E461" s="11"/>
     </row>
-    <row r="462" spans="1:5" ht="12.75" hidden="1">
+    <row r="462" spans="1:5" ht="12.75">
       <c r="A462" s="10"/>
       <c r="B462" s="10"/>
       <c r="E462" s="11"/>
     </row>
-    <row r="463" spans="1:5" ht="12.75" hidden="1">
+    <row r="463" spans="1:5" ht="12.75">
       <c r="A463" s="10"/>
       <c r="B463" s="10"/>
       <c r="E463" s="11"/>
     </row>
-    <row r="464" spans="1:5" ht="12.75" hidden="1">
+    <row r="464" spans="1:5" ht="12.75">
       <c r="A464" s="10"/>
       <c r="B464" s="10"/>
       <c r="E464" s="11"/>
     </row>
-    <row r="465" spans="1:5" ht="12.75" hidden="1">
+    <row r="465" spans="1:5" ht="12.75">
       <c r="A465" s="10"/>
       <c r="B465" s="10"/>
       <c r="E465" s="11"/>
     </row>
-    <row r="466" spans="1:5" ht="12.75" hidden="1">
+    <row r="466" spans="1:5" ht="12.75">
       <c r="A466" s="10"/>
       <c r="B466" s="10"/>
       <c r="E466" s="11"/>
     </row>
-    <row r="467" spans="1:5" ht="12.75" hidden="1">
+    <row r="467" spans="1:5" ht="12.75">
       <c r="A467" s="10"/>
       <c r="B467" s="10"/>
       <c r="E467" s="11"/>
     </row>
-    <row r="468" spans="1:5" ht="12.75" hidden="1">
+    <row r="468" spans="1:5" ht="12.75">
       <c r="A468" s="10"/>
       <c r="B468" s="10"/>
       <c r="E468" s="11"/>
     </row>
-    <row r="469" spans="1:5" ht="12.75" hidden="1">
+    <row r="469" spans="1:5" ht="12.75">
       <c r="A469" s="10"/>
       <c r="B469" s="10"/>
       <c r="E469" s="11"/>
     </row>
-    <row r="470" spans="1:5" ht="12.75" hidden="1">
+    <row r="470" spans="1:5" ht="12.75">
       <c r="A470" s="10"/>
       <c r="B470" s="10"/>
       <c r="E470" s="11"/>
     </row>
-    <row r="471" spans="1:5" ht="12.75" hidden="1">
+    <row r="471" spans="1:5" ht="12.75">
       <c r="A471" s="10"/>
       <c r="B471" s="10"/>
       <c r="E471" s="11"/>
     </row>
-    <row r="472" spans="1:5" ht="12.75" hidden="1">
+    <row r="472" spans="1:5" ht="12.75">
       <c r="A472" s="10"/>
       <c r="B472" s="10"/>
       <c r="E472" s="11"/>
     </row>
-    <row r="473" spans="1:5" ht="12.75" hidden="1">
+    <row r="473" spans="1:5" ht="12.75">
       <c r="A473" s="10"/>
       <c r="B473" s="10"/>
       <c r="E473" s="11"/>
     </row>
-    <row r="474" spans="1:5" ht="12.75" hidden="1">
+    <row r="474" spans="1:5" ht="12.75">
       <c r="A474" s="10"/>
       <c r="B474" s="10"/>
       <c r="E474" s="11"/>
     </row>
-    <row r="475" spans="1:5" ht="12.75" hidden="1">
+    <row r="475" spans="1:5" ht="12.75">
       <c r="A475" s="10"/>
       <c r="B475" s="10"/>
       <c r="E475" s="11"/>
     </row>
-    <row r="476" spans="1:5" ht="12.75" hidden="1">
+    <row r="476" spans="1:5" ht="12.75">
       <c r="A476" s="10"/>
       <c r="B476" s="10"/>
       <c r="E476" s="11"/>
     </row>
-    <row r="477" spans="1:5" ht="12.75" hidden="1">
+    <row r="477" spans="1:5" ht="12.75">
       <c r="A477" s="10"/>
       <c r="B477" s="10"/>
       <c r="E477" s="11"/>
     </row>
-    <row r="478" spans="1:5" ht="12.75" hidden="1">
+    <row r="478" spans="1:5" ht="12.75">
       <c r="A478" s="10"/>
       <c r="B478" s="10"/>
       <c r="E478" s="11"/>
     </row>
-    <row r="479" spans="1:5" ht="12.75" hidden="1">
+    <row r="479" spans="1:5" ht="12.75">
       <c r="A479" s="10"/>
       <c r="B479" s="10"/>
       <c r="E479" s="11"/>
     </row>
-    <row r="480" spans="1:5" ht="12.75" hidden="1">
+    <row r="480" spans="1:5" ht="12.75">
       <c r="A480" s="10"/>
       <c r="B480" s="10"/>
       <c r="E480" s="11"/>
     </row>
-    <row r="481" spans="1:5" ht="12.75" hidden="1">
+    <row r="481" spans="1:5" ht="12.75">
       <c r="A481" s="10"/>
       <c r="B481" s="10"/>
       <c r="E481" s="11"/>
     </row>
-    <row r="482" spans="1:5" ht="12.75" hidden="1">
+    <row r="482" spans="1:5" ht="12.75">
       <c r="A482" s="10"/>
       <c r="B482" s="10"/>
       <c r="E482" s="11"/>
     </row>
-    <row r="483" spans="1:5" ht="12.75" hidden="1">
+    <row r="483" spans="1:5" ht="12.75">
       <c r="A483" s="10"/>
       <c r="B483" s="10"/>
       <c r="E483" s="11"/>
     </row>
-    <row r="484" spans="1:5" ht="12.75" hidden="1">
+    <row r="484" spans="1:5" ht="12.75">
       <c r="A484" s="10"/>
       <c r="B484" s="10"/>
       <c r="E484" s="11"/>
     </row>
-    <row r="485" spans="1:5" ht="12.75" hidden="1">
+    <row r="485" spans="1:5" ht="12.75">
       <c r="A485" s="10"/>
       <c r="B485" s="10"/>
       <c r="E485" s="11"/>
     </row>
-    <row r="486" spans="1:5" ht="12.75" hidden="1">
+    <row r="486" spans="1:5" ht="12.75">
       <c r="A486" s="10"/>
       <c r="B486" s="10"/>
       <c r="E486" s="11"/>
     </row>
-    <row r="487" spans="1:5" ht="12.75" hidden="1">
+    <row r="487" spans="1:5" ht="12.75">
       <c r="A487" s="10"/>
       <c r="B487" s="10"/>
       <c r="E487" s="11"/>
     </row>
-    <row r="488" spans="1:5" ht="12.75" hidden="1">
+    <row r="488" spans="1:5" ht="12.75">
       <c r="A488" s="10"/>
       <c r="B488" s="10"/>
       <c r="E488" s="11"/>
     </row>
-    <row r="489" spans="1:5" ht="12.75" hidden="1">
+    <row r="489" spans="1:5" ht="12.75">
       <c r="A489" s="10"/>
       <c r="B489" s="10"/>
       <c r="E489" s="11"/>
     </row>
-    <row r="490" spans="1:5" ht="12.75" hidden="1">
+    <row r="490" spans="1:5" ht="12.75">
       <c r="A490" s="10"/>
       <c r="B490" s="10"/>
       <c r="E490" s="11"/>
     </row>
-    <row r="491" spans="1:5" ht="12.75" hidden="1">
+    <row r="491" spans="1:5" ht="12.75">
       <c r="A491" s="10"/>
       <c r="B491" s="10"/>
       <c r="E491" s="11"/>
     </row>
-    <row r="492" spans="1:5" ht="12.75" hidden="1">
+    <row r="492" spans="1:5" ht="12.75">
       <c r="A492" s="10"/>
       <c r="B492" s="10"/>
       <c r="E492" s="11"/>
     </row>
-    <row r="493" spans="1:5" ht="12.75" hidden="1">
+    <row r="493" spans="1:5" ht="12.75">
       <c r="A493" s="10"/>
       <c r="B493" s="10"/>
       <c r="E493" s="11"/>
     </row>
-    <row r="494" spans="1:5" ht="12.75" hidden="1">
+    <row r="494" spans="1:5" ht="12.75">
       <c r="A494" s="10"/>
       <c r="B494" s="10"/>
       <c r="E494" s="11"/>
     </row>
-    <row r="495" spans="1:5" ht="12.75" hidden="1">
+    <row r="495" spans="1:5" ht="12.75">
       <c r="A495" s="10"/>
       <c r="B495" s="10"/>
       <c r="E495" s="11"/>
     </row>
-    <row r="496" spans="1:5" ht="12.75" hidden="1">
+    <row r="496" spans="1:5" ht="12.75">
       <c r="A496" s="10"/>
       <c r="B496" s="10"/>
       <c r="E496" s="11"/>
     </row>
-    <row r="497" spans="1:5" ht="12.75" hidden="1">
+    <row r="497" spans="1:5" ht="12.75">
       <c r="A497" s="10"/>
       <c r="B497" s="10"/>
       <c r="E497" s="11"/>
     </row>
-    <row r="498" spans="1:5" ht="12.75" hidden="1">
+    <row r="498" spans="1:5" ht="12.75">
       <c r="A498" s="10"/>
       <c r="B498" s="10"/>
       <c r="E498" s="11"/>
     </row>
-    <row r="499" spans="1:5" ht="12.75" hidden="1">
+    <row r="499" spans="1:5" ht="12.75">
       <c r="A499" s="10"/>
       <c r="B499" s="10"/>
       <c r="E499" s="11"/>
     </row>
-    <row r="500" spans="1:5" ht="12.75" hidden="1">
+    <row r="500" spans="1:5" ht="12.75">
       <c r="A500" s="10"/>
       <c r="B500" s="10"/>
       <c r="E500" s="11"/>
     </row>
-    <row r="501" spans="1:5" ht="12.75" hidden="1">
+    <row r="501" spans="1:5" ht="12.75">
       <c r="A501" s="10"/>
       <c r="B501" s="10"/>
       <c r="E501" s="11"/>
     </row>
-    <row r="502" spans="1:5" ht="12.75" hidden="1">
+    <row r="502" spans="1:5" ht="12.75">
       <c r="A502" s="10"/>
       <c r="B502" s="10"/>
       <c r="E502" s="11"/>
     </row>
-    <row r="503" spans="1:5" ht="12.75" hidden="1">
+    <row r="503" spans="1:5" ht="12.75">
       <c r="A503" s="10"/>
       <c r="B503" s="10"/>
       <c r="E503" s="11"/>
     </row>
-    <row r="504" spans="1:5" ht="12.75" hidden="1">
+    <row r="504" spans="1:5" ht="12.75">
       <c r="A504" s="10"/>
       <c r="B504" s="10"/>
       <c r="E504" s="11"/>
     </row>
-    <row r="505" spans="1:5" ht="12.75" hidden="1">
+    <row r="505" spans="1:5" ht="12.75">
       <c r="A505" s="10"/>
       <c r="B505" s="10"/>
       <c r="E505" s="11"/>
     </row>
-    <row r="506" spans="1:5" ht="12.75" hidden="1">
+    <row r="506" spans="1:5" ht="12.75">
       <c r="A506" s="10"/>
       <c r="B506" s="10"/>
       <c r="E506" s="11"/>
     </row>
-    <row r="507" spans="1:5" ht="12.75" hidden="1">
+    <row r="507" spans="1:5" ht="12.75">
       <c r="A507" s="10"/>
       <c r="B507" s="10"/>
       <c r="E507" s="11"/>
     </row>
-    <row r="508" spans="1:5" ht="12.75" hidden="1">
+    <row r="508" spans="1:5" ht="12.75">
       <c r="A508" s="10"/>
       <c r="B508" s="10"/>
       <c r="E508" s="11"/>
     </row>
-    <row r="509" spans="1:5" ht="12.75" hidden="1">
+    <row r="509" spans="1:5" ht="12.75">
       <c r="A509" s="10"/>
       <c r="B509" s="10"/>
       <c r="E509" s="11"/>
     </row>
-    <row r="510" spans="1:5" ht="12.75" hidden="1">
+    <row r="510" spans="1:5" ht="12.75">
       <c r="A510" s="10"/>
       <c r="B510" s="10"/>
       <c r="E510" s="11"/>
     </row>
-    <row r="511" spans="1:5" ht="12.75" hidden="1">
+    <row r="511" spans="1:5" ht="12.75">
       <c r="A511" s="10"/>
       <c r="B511" s="10"/>
       <c r="E511" s="11"/>
     </row>
-    <row r="512" spans="1:5" ht="12.75" hidden="1">
+    <row r="512" spans="1:5" ht="12.75">
       <c r="A512" s="10"/>
       <c r="B512" s="10"/>
       <c r="E512" s="11"/>
     </row>
-    <row r="513" spans="1:5" ht="12.75" hidden="1">
+    <row r="513" spans="1:5" ht="12.75">
       <c r="A513" s="10"/>
       <c r="B513" s="10"/>
       <c r="E513" s="11"/>
     </row>
-    <row r="514" spans="1:5" ht="12.75" hidden="1">
+    <row r="514" spans="1:5" ht="12.75">
       <c r="A514" s="10"/>
       <c r="B514" s="10"/>
       <c r="E514" s="11"/>
     </row>
-    <row r="515" spans="1:5" ht="12.75" hidden="1">
+    <row r="515" spans="1:5" ht="12.75">
       <c r="A515" s="10"/>
       <c r="B515" s="10"/>
       <c r="E515" s="11"/>
     </row>
-    <row r="516" spans="1:5" ht="12.75" hidden="1">
+    <row r="516" spans="1:5" ht="12.75">
       <c r="A516" s="10"/>
       <c r="B516" s="10"/>
       <c r="E516" s="11"/>
     </row>
-    <row r="517" spans="1:5" ht="12.75" hidden="1">
+    <row r="517" spans="1:5" ht="12.75">
       <c r="A517" s="10"/>
       <c r="B517" s="10"/>
       <c r="E517" s="11"/>
     </row>
-    <row r="518" spans="1:5" ht="12.75" hidden="1">
+    <row r="518" spans="1:5" ht="12.75">
       <c r="A518" s="10"/>
       <c r="B518" s="10"/>
       <c r="E518" s="11"/>
     </row>
-    <row r="519" spans="1:5" ht="12.75" hidden="1">
+    <row r="519" spans="1:5" ht="12.75">
       <c r="A519" s="10"/>
       <c r="B519" s="10"/>
       <c r="E519" s="11"/>
     </row>
-    <row r="520" spans="1:5" ht="12.75" hidden="1">
+    <row r="520" spans="1:5" ht="12.75">
       <c r="A520" s="10"/>
       <c r="B520" s="10"/>
       <c r="E520" s="11"/>
     </row>
-    <row r="521" spans="1:5" ht="12.75" hidden="1">
+    <row r="521" spans="1:5" ht="12.75">
       <c r="A521" s="10"/>
       <c r="B521" s="10"/>
       <c r="E521" s="11"/>
     </row>
-    <row r="522" spans="1:5" ht="12.75" hidden="1">
+    <row r="522" spans="1:5" ht="12.75">
       <c r="A522" s="10"/>
       <c r="B522" s="10"/>
       <c r="E522" s="11"/>
     </row>
-    <row r="523" spans="1:5" ht="12.75" hidden="1">
+    <row r="523" spans="1:5" ht="12.75">
       <c r="A523" s="10"/>
       <c r="B523" s="10"/>
       <c r="E523" s="11"/>
     </row>
-    <row r="524" spans="1:5" ht="12.75" hidden="1">
+    <row r="524" spans="1:5" ht="12.75">
       <c r="A524" s="10"/>
       <c r="B524" s="10"/>
       <c r="E524" s="11"/>
     </row>
-    <row r="525" spans="1:5" ht="12.75" hidden="1">
+    <row r="525" spans="1:5" ht="12.75">
       <c r="A525" s="10"/>
       <c r="B525" s="10"/>
       <c r="E525" s="11"/>
     </row>
-    <row r="526" spans="1:5" ht="12.75" hidden="1">
+    <row r="526" spans="1:5" ht="12.75">
       <c r="A526" s="10"/>
       <c r="B526" s="10"/>
       <c r="E526" s="11"/>
     </row>
-    <row r="527" spans="1:5" ht="12.75" hidden="1">
+    <row r="527" spans="1:5" ht="12.75">
       <c r="A527" s="10"/>
       <c r="B527" s="10"/>
       <c r="E527" s="11"/>
     </row>
-    <row r="528" spans="1:5" ht="12.75" hidden="1">
+    <row r="528" spans="1:5" ht="12.75">
       <c r="A528" s="10"/>
       <c r="B528" s="10"/>
       <c r="E528" s="11"/>
     </row>
-    <row r="529" spans="1:5" ht="12.75" hidden="1">
+    <row r="529" spans="1:5" ht="12.75">
       <c r="A529" s="10"/>
       <c r="B529" s="10"/>
       <c r="E529" s="11"/>
     </row>
-    <row r="530" spans="1:5" ht="12.75" hidden="1">
+    <row r="530" spans="1:5" ht="12.75">
       <c r="A530" s="10"/>
       <c r="B530" s="10"/>
       <c r="E530" s="11"/>
     </row>
-    <row r="531" spans="1:5" ht="12.75" hidden="1">
+    <row r="531" spans="1:5" ht="12.75">
       <c r="A531" s="10"/>
       <c r="B531" s="10"/>
       <c r="E531" s="11"/>
     </row>
-    <row r="532" spans="1:5" ht="12.75" hidden="1">
+    <row r="532" spans="1:5" ht="12.75">
       <c r="A532" s="10"/>
       <c r="B532" s="10"/>
       <c r="E532" s="11"/>
     </row>
-    <row r="533" spans="1:5" ht="12.75" hidden="1">
+    <row r="533" spans="1:5" ht="12.75">
       <c r="A533" s="10"/>
       <c r="B533" s="10"/>
       <c r="E533" s="11"/>
     </row>
-    <row r="534" spans="1:5" ht="12.75" hidden="1">
+    <row r="534" spans="1:5" ht="12.75">
       <c r="A534" s="10"/>
       <c r="B534" s="10"/>
       <c r="E534" s="11"/>
     </row>
-    <row r="535" spans="1:5" ht="12.75" hidden="1">
+    <row r="535" spans="1:5" ht="12.75">
       <c r="A535" s="10"/>
       <c r="B535" s="10"/>
       <c r="E535" s="11"/>
     </row>
-    <row r="536" spans="1:5" ht="12.75" hidden="1">
+    <row r="536" spans="1:5" ht="12.75">
       <c r="A536" s="10"/>
       <c r="B536" s="10"/>
       <c r="E536" s="11"/>
     </row>
-    <row r="537" spans="1:5" ht="12.75" hidden="1">
+    <row r="537" spans="1:5" ht="12.75">
       <c r="A537" s="10"/>
       <c r="B537" s="10"/>
       <c r="E537" s="11"/>
     </row>
-    <row r="538" spans="1:5" ht="12.75" hidden="1">
+    <row r="538" spans="1:5" ht="12.75">
       <c r="A538" s="10"/>
       <c r="B538" s="10"/>
       <c r="E538" s="11"/>
     </row>
-    <row r="539" spans="1:5" ht="12.75" hidden="1">
+    <row r="539" spans="1:5" ht="12.75">
       <c r="A539" s="10"/>
       <c r="B539" s="10"/>
       <c r="E539" s="11"/>
     </row>
-    <row r="540" spans="1:5" ht="12.75" hidden="1">
+    <row r="540" spans="1:5" ht="12.75">
       <c r="A540" s="10"/>
       <c r="B540" s="10"/>
       <c r="E540" s="11"/>
     </row>
-    <row r="541" spans="1:5" ht="12.75" hidden="1">
+    <row r="541" spans="1:5" ht="12.75">
       <c r="A541" s="10"/>
       <c r="B541" s="10"/>
       <c r="E541" s="11"/>
     </row>
-    <row r="542" spans="1:5" ht="12.75" hidden="1">
+    <row r="542" spans="1:5" ht="12.75">
       <c r="A542" s="10"/>
       <c r="B542" s="10"/>
       <c r="E542" s="11"/>
     </row>
-    <row r="543" spans="1:5" ht="12.75" hidden="1">
+    <row r="543" spans="1:5" ht="12.75">
       <c r="A543" s="10"/>
       <c r="B543" s="10"/>
       <c r="E543" s="11"/>
     </row>
-    <row r="544" spans="1:5" ht="12.75" hidden="1">
+    <row r="544" spans="1:5" ht="12.75">
       <c r="A544" s="10"/>
       <c r="B544" s="10"/>
       <c r="E544" s="11"/>
     </row>
-    <row r="545" spans="1:5" ht="12.75" hidden="1">
+    <row r="545" spans="1:5" ht="12.75">
       <c r="A545" s="10"/>
       <c r="B545" s="10"/>
       <c r="E545" s="11"/>
     </row>
-    <row r="546" spans="1:5" ht="12.75" hidden="1">
+    <row r="546" spans="1:5" ht="12.75">
       <c r="A546" s="10"/>
       <c r="B546" s="10"/>
       <c r="E546" s="11"/>
     </row>
-    <row r="547" spans="1:5" ht="12.75" hidden="1">
+    <row r="547" spans="1:5" ht="12.75">
       <c r="A547" s="10"/>
       <c r="B547" s="10"/>
       <c r="E547" s="11"/>
     </row>
-    <row r="548" spans="1:5" ht="12.75" hidden="1">
+    <row r="548" spans="1:5" ht="12.75">
       <c r="A548" s="10"/>
       <c r="B548" s="10"/>
       <c r="E548" s="11"/>
     </row>
-    <row r="549" spans="1:5" ht="12.75" hidden="1">
+    <row r="549" spans="1:5" ht="12.75">
       <c r="A549" s="10"/>
       <c r="B549" s="10"/>
       <c r="E549" s="11"/>
     </row>
-    <row r="550" spans="1:5" ht="12.75" hidden="1">
+    <row r="550" spans="1:5" ht="12.75">
       <c r="A550" s="10"/>
       <c r="B550" s="10"/>
       <c r="E550" s="11"/>
     </row>
-    <row r="551" spans="1:5" ht="12.75" hidden="1">
+    <row r="551" spans="1:5" ht="12.75">
       <c r="A551" s="10"/>
       <c r="B551" s="10"/>
       <c r="E551" s="11"/>
     </row>
-    <row r="552" spans="1:5" ht="12.75" hidden="1">
+    <row r="552" spans="1:5" ht="12.75">
       <c r="A552" s="10"/>
       <c r="B552" s="10"/>
       <c r="E552" s="11"/>
     </row>
-    <row r="553" spans="1:5" ht="12.75" hidden="1">
+    <row r="553" spans="1:5" ht="12.75">
       <c r="A553" s="10"/>
       <c r="B553" s="10"/>
       <c r="E553" s="11"/>
     </row>
-    <row r="554" spans="1:5" ht="12.75" hidden="1">
+    <row r="554" spans="1:5" ht="12.75">
       <c r="A554" s="10"/>
       <c r="B554" s="10"/>
       <c r="E554" s="11"/>
     </row>
-    <row r="555" spans="1:5" ht="12.75" hidden="1">
+    <row r="555" spans="1:5" ht="12.75">
       <c r="A555" s="10"/>
       <c r="B555" s="10"/>
       <c r="E555" s="11"/>
     </row>
-    <row r="556" spans="1:5" ht="12.75" hidden="1">
+    <row r="556" spans="1:5" ht="12.75">
       <c r="A556" s="10"/>
       <c r="B556" s="10"/>
       <c r="E556" s="11"/>
     </row>
-    <row r="557" spans="1:5" ht="12.75" hidden="1">
+    <row r="557" spans="1:5" ht="12.75">
       <c r="A557" s="10"/>
       <c r="B557" s="10"/>
       <c r="E557" s="11"/>
     </row>
-    <row r="558" spans="1:5" ht="12.75" hidden="1">
+    <row r="558" spans="1:5" ht="12.75">
       <c r="A558" s="10"/>
       <c r="B558" s="10"/>
       <c r="E558" s="11"/>
     </row>
-    <row r="559" spans="1:5" ht="12.75" hidden="1">
+    <row r="559" spans="1:5" ht="12.75">
       <c r="A559" s="10"/>
       <c r="B559" s="10"/>
       <c r="E559" s="11"/>
     </row>
-    <row r="560" spans="1:5" ht="12.75" hidden="1">
+    <row r="560" spans="1:5" ht="12.75">
       <c r="A560" s="10"/>
       <c r="B560" s="10"/>
       <c r="E560" s="11"/>
     </row>
-    <row r="561" spans="1:5" ht="12.75" hidden="1">
+    <row r="561" spans="1:5" ht="12.75">
       <c r="A561" s="10"/>
       <c r="B561" s="10"/>
       <c r="E561" s="11"/>
     </row>
-    <row r="562" spans="1:5" ht="12.75" hidden="1">
+    <row r="562" spans="1:5" ht="12.75">
       <c r="A562" s="10"/>
       <c r="B562" s="10"/>
       <c r="E562" s="11"/>
     </row>
-    <row r="563" spans="1:5" ht="12.75" hidden="1">
+    <row r="563" spans="1:5" ht="12.75">
       <c r="A563" s="10"/>
       <c r="B563" s="10"/>
       <c r="E563" s="11"/>
     </row>
-    <row r="564" spans="1:5" ht="12.75" hidden="1">
+    <row r="564" spans="1:5" ht="12.75">
       <c r="A564" s="10"/>
       <c r="B564" s="10"/>
       <c r="E564" s="11"/>
     </row>
-    <row r="565" spans="1:5" ht="12.75" hidden="1">
+    <row r="565" spans="1:5" ht="12.75">
       <c r="A565" s="10"/>
       <c r="B565" s="10"/>
       <c r="E565" s="11"/>
     </row>
-    <row r="566" spans="1:5" ht="12.75" hidden="1">
+    <row r="566" spans="1:5" ht="12.75">
       <c r="A566" s="10"/>
       <c r="B566" s="10"/>
       <c r="E566" s="11"/>
     </row>
-    <row r="567" spans="1:5" ht="12.75" hidden="1">
+    <row r="567" spans="1:5" ht="12.75">
       <c r="A567" s="10"/>
       <c r="B567" s="10"/>
       <c r="E567" s="11"/>
     </row>
-    <row r="568" spans="1:5" ht="12.75" hidden="1">
+    <row r="568" spans="1:5" ht="12.75">
       <c r="A568" s="10"/>
       <c r="B568" s="10"/>
       <c r="E568" s="11"/>
     </row>
-    <row r="569" spans="1:5" ht="12.75" hidden="1">
+    <row r="569" spans="1:5" ht="12.75">
       <c r="A569" s="10"/>
       <c r="B569" s="10"/>
       <c r="E569" s="11"/>
     </row>
-    <row r="570" spans="1:5" ht="12.75" hidden="1">
+    <row r="570" spans="1:5" ht="12.75">
       <c r="A570" s="10"/>
       <c r="B570" s="10"/>
       <c r="E570" s="11"/>
     </row>
-    <row r="571" spans="1:5" ht="12.75" hidden="1">
+    <row r="571" spans="1:5" ht="12.75">
       <c r="A571" s="10"/>
       <c r="B571" s="10"/>
       <c r="E571" s="11"/>
     </row>
-    <row r="572" spans="1:5" ht="12.75" hidden="1">
+    <row r="572" spans="1:5" ht="12.75">
       <c r="A572" s="10"/>
       <c r="B572" s="10"/>
       <c r="E572" s="11"/>
     </row>
-    <row r="573" spans="1:5" ht="12.75" hidden="1">
+    <row r="573" spans="1:5" ht="12.75">
       <c r="A573" s="10"/>
       <c r="B573" s="10"/>
       <c r="E573" s="11"/>
     </row>
-    <row r="574" spans="1:5" ht="12.75" hidden="1">
+    <row r="574" spans="1:5" ht="12.75">
       <c r="A574" s="10"/>
       <c r="B574" s="10"/>
       <c r="E574" s="11"/>
     </row>
-    <row r="575" spans="1:5" ht="12.75" hidden="1">
+    <row r="575" spans="1:5" ht="12.75">
       <c r="A575" s="10"/>
       <c r="B575" s="10"/>
       <c r="E575" s="11"/>
     </row>
-    <row r="576" spans="1:5" ht="12.75" hidden="1">
+    <row r="576" spans="1:5" ht="12.75">
       <c r="A576" s="10"/>
       <c r="B576" s="10"/>
       <c r="E576" s="11"/>
     </row>
-    <row r="577" spans="1:5" ht="12.75" hidden="1">
+    <row r="577" spans="1:5" ht="12.75">
       <c r="A577" s="10"/>
       <c r="B577" s="10"/>
       <c r="E577" s="11"/>
     </row>
-    <row r="578" spans="1:5" ht="12.75" hidden="1">
+    <row r="578" spans="1:5" ht="12.75">
       <c r="A578" s="10"/>
       <c r="B578" s="10"/>
       <c r="E578" s="11"/>
     </row>
-    <row r="579" spans="1:5" ht="12.75" hidden="1">
+    <row r="579" spans="1:5" ht="12.75">
       <c r="A579" s="10"/>
       <c r="B579" s="10"/>
       <c r="E579" s="11"/>
     </row>
-    <row r="580" spans="1:5" ht="12.75" hidden="1">
+    <row r="580" spans="1:5" ht="12.75">
       <c r="A580" s="10"/>
       <c r="B580" s="10"/>
       <c r="E580" s="11"/>
     </row>
-    <row r="581" spans="1:5" ht="12.75" hidden="1">
+    <row r="581" spans="1:5" ht="12.75">
       <c r="A581" s="10"/>
       <c r="B581" s="10"/>
       <c r="E581" s="11"/>
     </row>
-    <row r="582" spans="1:5" ht="12.75" hidden="1">
+    <row r="582" spans="1:5" ht="12.75">
       <c r="A582" s="10"/>
       <c r="B582" s="10"/>
       <c r="E582" s="11"/>
     </row>
-    <row r="583" spans="1:5" ht="12.75" hidden="1">
+    <row r="583" spans="1:5" ht="12.75">
       <c r="A583" s="10"/>
       <c r="B583" s="10"/>
       <c r="E583" s="11"/>
     </row>
-    <row r="584" spans="1:5" ht="12.75" hidden="1">
+    <row r="584" spans="1:5" ht="12.75">
       <c r="A584" s="10"/>
       <c r="B584" s="10"/>
       <c r="E584" s="11"/>
     </row>
-    <row r="585" spans="1:5" ht="12.75" hidden="1">
+    <row r="585" spans="1:5" ht="12.75">
       <c r="A585" s="10"/>
       <c r="B585" s="10"/>
       <c r="E585" s="11"/>
     </row>
-    <row r="586" spans="1:5" ht="12.75" hidden="1">
+    <row r="586" spans="1:5" ht="12.75">
       <c r="A586" s="10"/>
       <c r="B586" s="10"/>
       <c r="E586" s="11"/>
     </row>
-    <row r="587" spans="1:5" ht="12.75" hidden="1">
+    <row r="587" spans="1:5" ht="12.75">
       <c r="A587" s="10"/>
       <c r="B587" s="10"/>
       <c r="E587" s="11"/>
     </row>
-    <row r="588" spans="1:5" ht="12.75" hidden="1">
+    <row r="588" spans="1:5" ht="12.75">
       <c r="A588" s="10"/>
       <c r="B588" s="10"/>
       <c r="E588" s="11"/>
     </row>
-    <row r="589" spans="1:5" ht="12.75" hidden="1">
+    <row r="589" spans="1:5" ht="12.75">
       <c r="A589" s="10"/>
       <c r="B589" s="10"/>
       <c r="E589" s="11"/>
     </row>
-    <row r="590" spans="1:5" ht="12.75" hidden="1">
+    <row r="590" spans="1:5" ht="12.75">
       <c r="A590" s="10"/>
       <c r="B590" s="10"/>
       <c r="E590" s="11"/>
     </row>
-    <row r="591" spans="1:5" ht="12.75" hidden="1">
+    <row r="591" spans="1:5" ht="12.75">
       <c r="A591" s="10"/>
       <c r="B591" s="10"/>
       <c r="E591" s="11"/>
     </row>
-    <row r="592" spans="1:5" ht="12.75" hidden="1">
+    <row r="592" spans="1:5" ht="12.75">
       <c r="A592" s="10"/>
       <c r="B592" s="10"/>
       <c r="E592" s="11"/>
     </row>
-    <row r="593" spans="1:5" ht="12.75" hidden="1">
+    <row r="593" spans="1:5" ht="12.75">
       <c r="A593" s="10"/>
       <c r="B593" s="10"/>
       <c r="E593" s="11"/>
     </row>
-    <row r="594" spans="1:5" ht="12.75" hidden="1">
+    <row r="594" spans="1:5" ht="12.75">
       <c r="A594" s="10"/>
       <c r="B594" s="10"/>
       <c r="E594" s="11"/>
     </row>
-    <row r="595" spans="1:5" ht="12.75" hidden="1">
+    <row r="595" spans="1:5" ht="12.75">
       <c r="A595" s="10"/>
       <c r="B595" s="10"/>
       <c r="E595" s="11"/>
     </row>
-    <row r="596" spans="1:5" ht="12.75" hidden="1">
+    <row r="596" spans="1:5" ht="12.75">
       <c r="A596" s="10"/>
       <c r="B596" s="10"/>
       <c r="E596" s="11"/>
     </row>
-    <row r="597" spans="1:5" ht="12.75" hidden="1">
+    <row r="597" spans="1:5" ht="12.75">
       <c r="A597" s="10"/>
       <c r="B597" s="10"/>
       <c r="E597" s="11"/>
     </row>
-    <row r="598" spans="1:5" ht="12.75" hidden="1">
+    <row r="598" spans="1:5" ht="12.75">
       <c r="A598" s="10"/>
       <c r="B598" s="10"/>
       <c r="E598" s="11"/>
     </row>
-    <row r="599" spans="1:5" ht="12.75" hidden="1">
+    <row r="599" spans="1:5" ht="12.75">
       <c r="A599" s="10"/>
       <c r="B599" s="10"/>
       <c r="E599" s="11"/>
     </row>
-    <row r="600" spans="1:5" ht="12.75" hidden="1">
+    <row r="600" spans="1:5" ht="12.75">
       <c r="A600" s="10"/>
       <c r="B600" s="10"/>
       <c r="E600" s="11"/>
     </row>
-    <row r="601" spans="1:5" ht="12.75" hidden="1">
+    <row r="601" spans="1:5" ht="12.75">
       <c r="A601" s="10"/>
       <c r="B601" s="10"/>
       <c r="E601" s="11"/>
     </row>
-    <row r="602" spans="1:5" ht="12.75" hidden="1">
+    <row r="602" spans="1:5" ht="12.75">
       <c r="A602" s="10"/>
       <c r="B602" s="10"/>
       <c r="E602" s="11"/>
     </row>
-    <row r="603" spans="1:5" ht="12.75" hidden="1">
+    <row r="603" spans="1:5" ht="12.75">
       <c r="A603" s="10"/>
       <c r="B603" s="10"/>
       <c r="E603" s="11"/>
     </row>
-    <row r="604" spans="1:5" ht="12.75" hidden="1">
+    <row r="604" spans="1:5" ht="12.75">
       <c r="A604" s="10"/>
       <c r="B604" s="10"/>
       <c r="E604" s="11"/>
     </row>
-    <row r="605" spans="1:5" ht="12.75" hidden="1">
+    <row r="605" spans="1:5" ht="12.75">
       <c r="A605" s="10"/>
       <c r="B605" s="10"/>
       <c r="E605" s="11"/>
     </row>
-    <row r="606" spans="1:5" ht="12.75" hidden="1">
+    <row r="606" spans="1:5" ht="12.75">
       <c r="A606" s="10"/>
       <c r="B606" s="10"/>
       <c r="E606" s="11"/>
     </row>
-    <row r="607" spans="1:5" ht="12.75" hidden="1">
+    <row r="607" spans="1:5" ht="12.75">
       <c r="A607" s="10"/>
       <c r="B607" s="10"/>
       <c r="E607" s="11"/>
     </row>
-    <row r="608" spans="1:5" ht="12.75" hidden="1">
+    <row r="608" spans="1:5" ht="12.75">
       <c r="A608" s="10"/>
       <c r="B608" s="10"/>
       <c r="E608" s="11"/>
     </row>
-    <row r="609" spans="1:5" ht="12.75" hidden="1">
+    <row r="609" spans="1:5" ht="12.75">
       <c r="A609" s="10"/>
       <c r="B609" s="10"/>
       <c r="E609" s="11"/>
     </row>
-    <row r="610" spans="1:5" ht="12.75" hidden="1">
+    <row r="610" spans="1:5" ht="12.75">
       <c r="A610" s="10"/>
       <c r="B610" s="10"/>
       <c r="E610" s="11"/>
     </row>
-    <row r="611" spans="1:5" ht="12.75" hidden="1">
+    <row r="611" spans="1:5" ht="12.75">
       <c r="A611" s="10"/>
       <c r="B611" s="10"/>
       <c r="E611" s="11"/>
     </row>
-    <row r="612" spans="1:5" ht="12.75" hidden="1">
+    <row r="612" spans="1:5" ht="12.75">
       <c r="A612" s="10"/>
       <c r="B612" s="10"/>
       <c r="E612" s="11"/>
     </row>
-    <row r="613" spans="1:5" ht="12.75" hidden="1">
+    <row r="613" spans="1:5" ht="12.75">
       <c r="A613" s="10"/>
       <c r="B613" s="10"/>
       <c r="E613" s="11"/>
     </row>
-    <row r="614" spans="1:5" ht="12.75" hidden="1">
+    <row r="614" spans="1:5" ht="12.75">
       <c r="A614" s="10"/>
       <c r="B614" s="10"/>
       <c r="E614" s="11"/>
     </row>
-    <row r="615" spans="1:5" ht="12.75" hidden="1">
+    <row r="615" spans="1:5" ht="12.75">
       <c r="A615" s="10"/>
       <c r="B615" s="10"/>
       <c r="E615" s="11"/>
     </row>
-    <row r="616" spans="1:5" ht="12.75" hidden="1">
+    <row r="616" spans="1:5" ht="12.75">
       <c r="A616" s="10"/>
       <c r="B616" s="10"/>
       <c r="E616" s="11"/>
     </row>
-    <row r="617" spans="1:5" ht="12.75" hidden="1">
+    <row r="617" spans="1:5" ht="12.75">
       <c r="A617" s="10"/>
       <c r="B617" s="10"/>
       <c r="E617" s="11"/>
     </row>
-    <row r="618" spans="1:5" ht="12.75" hidden="1">
+    <row r="618" spans="1:5" ht="12.75">
       <c r="A618" s="10"/>
       <c r="B618" s="10"/>
       <c r="E618" s="11"/>
     </row>
-    <row r="619" spans="1:5" ht="12.75" hidden="1">
+    <row r="619" spans="1:5" ht="12.75">
       <c r="A619" s="10"/>
       <c r="B619" s="10"/>
       <c r="E619" s="11"/>
     </row>
-    <row r="620" spans="1:5" ht="12.75" hidden="1">
+    <row r="620" spans="1:5" ht="12.75">
       <c r="A620" s="10"/>
       <c r="B620" s="10"/>
       <c r="E620" s="11"/>
     </row>
-    <row r="621" spans="1:5" ht="12.75" hidden="1">
+    <row r="621" spans="1:5" ht="12.75">
       <c r="A621" s="10"/>
       <c r="B621" s="10"/>
       <c r="E621" s="11"/>
     </row>
-    <row r="622" spans="1:5" ht="12.75" hidden="1">
+    <row r="622" spans="1:5" ht="12.75">
       <c r="A622" s="10"/>
       <c r="B622" s="10"/>
       <c r="E622" s="11"/>
     </row>
-    <row r="623" spans="1:5" ht="12.75" hidden="1">
+    <row r="623" spans="1:5" ht="12.75">
       <c r="A623" s="10"/>
       <c r="B623" s="10"/>
       <c r="E623" s="11"/>
     </row>
-    <row r="624" spans="1:5" ht="12.75" hidden="1">
+    <row r="624" spans="1:5" ht="12.75">
       <c r="A624" s="10"/>
       <c r="B624" s="10"/>
       <c r="E624" s="11"/>
     </row>
-    <row r="625" spans="1:5" ht="12.75" hidden="1">
+    <row r="625" spans="1:5" ht="12.75">
       <c r="A625" s="10"/>
       <c r="B625" s="10"/>
       <c r="E625" s="11"/>
     </row>
-    <row r="626" spans="1:5" ht="12.75" hidden="1">
+    <row r="626" spans="1:5" ht="12.75">
       <c r="A626" s="10"/>
       <c r="B626" s="10"/>
       <c r="E626" s="11"/>
     </row>
-    <row r="627" spans="1:5" ht="12.75" hidden="1">
+    <row r="627" spans="1:5" ht="12.75">
       <c r="A627" s="10"/>
       <c r="B627" s="10"/>
       <c r="E627" s="11"/>
     </row>
-    <row r="628" spans="1:5" ht="12.75" hidden="1">
+    <row r="628" spans="1:5" ht="12.75">
       <c r="A628" s="10"/>
       <c r="B628" s="10"/>
       <c r="E628" s="11"/>
     </row>
-    <row r="629" spans="1:5" ht="12.75" hidden="1">
+    <row r="629" spans="1:5" ht="12.75">
       <c r="A629" s="10"/>
       <c r="B629" s="10"/>
       <c r="E629" s="11"/>
     </row>
-    <row r="630" spans="1:5" ht="12.75" hidden="1">
+    <row r="630" spans="1:5" ht="12.75">
       <c r="A630" s="10"/>
       <c r="B630" s="10"/>
       <c r="E630" s="11"/>
     </row>
-    <row r="631" spans="1:5" ht="12.75" hidden="1">
+    <row r="631" spans="1:5" ht="12.75">
       <c r="A631" s="10"/>
       <c r="B631" s="10"/>
       <c r="E631" s="11"/>
     </row>
-    <row r="632" spans="1:5" ht="12.75" hidden="1">
+    <row r="632" spans="1:5" ht="12.75">
       <c r="A632" s="10"/>
       <c r="B632" s="10"/>
       <c r="E632" s="11"/>
     </row>
-    <row r="633" spans="1:5" ht="12.75" hidden="1">
+    <row r="633" spans="1:5" ht="12.75">
       <c r="A633" s="10"/>
       <c r="B633" s="10"/>
       <c r="E633" s="11"/>
     </row>
-    <row r="634" spans="1:5" ht="12.75" hidden="1">
+    <row r="634" spans="1:5" ht="12.75">
       <c r="A634" s="10"/>
       <c r="B634" s="10"/>
       <c r="E634" s="11"/>
     </row>
-    <row r="635" spans="1:5" ht="12.75" hidden="1">
+    <row r="635" spans="1:5" ht="12.75">
       <c r="A635" s="10"/>
       <c r="B635" s="10"/>
       <c r="E635" s="11"/>
     </row>
-    <row r="636" spans="1:5" ht="12.75" hidden="1">
+    <row r="636" spans="1:5" ht="12.75">
       <c r="A636" s="10"/>
       <c r="B636" s="10"/>
       <c r="E636" s="11"/>
     </row>
-    <row r="637" spans="1:5" ht="12.75" hidden="1">
+    <row r="637" spans="1:5" ht="12.75">
       <c r="A637" s="10"/>
       <c r="B637" s="10"/>
       <c r="E637" s="11"/>
     </row>
-    <row r="638" spans="1:5" ht="12.75" hidden="1">
+    <row r="638" spans="1:5" ht="12.75">
       <c r="A638" s="10"/>
       <c r="B638" s="10"/>
       <c r="E638" s="11"/>
     </row>
-    <row r="639" spans="1:5" ht="12.75" hidden="1">
+    <row r="639" spans="1:5" ht="12.75">
       <c r="A639" s="10"/>
       <c r="B639" s="10"/>
       <c r="E639" s="11"/>
     </row>
-    <row r="640" spans="1:5" ht="12.75" hidden="1">
+    <row r="640" spans="1:5" ht="12.75">
       <c r="A640" s="10"/>
       <c r="B640" s="10"/>
       <c r="E640" s="11"/>
     </row>
-    <row r="641" spans="1:5" ht="12.75" hidden="1">
+    <row r="641" spans="1:5" ht="12.75">
       <c r="A641" s="10"/>
       <c r="B641" s="10"/>
       <c r="E641" s="11"/>
     </row>
-    <row r="642" spans="1:5" ht="12.75" hidden="1">
+    <row r="642" spans="1:5" ht="12.75">
       <c r="A642" s="10"/>
       <c r="B642" s="10"/>
       <c r="E642" s="11"/>
     </row>
-    <row r="643" spans="1:5" ht="12.75" hidden="1">
+    <row r="643" spans="1:5" ht="12.75">
       <c r="A643" s="10"/>
       <c r="B643" s="10"/>
       <c r="E643" s="11"/>
     </row>
-    <row r="644" spans="1:5" ht="12.75" hidden="1">
+    <row r="644" spans="1:5" ht="12.75">
       <c r="A644" s="10"/>
       <c r="B644" s="10"/>
       <c r="E644" s="11"/>
     </row>
-    <row r="645" spans="1:5" ht="12.75" hidden="1">
+    <row r="645" spans="1:5" ht="12.75">
       <c r="A645" s="10"/>
       <c r="B645" s="10"/>
       <c r="E645" s="11"/>
     </row>
-    <row r="646" spans="1:5" ht="12.75" hidden="1">
+    <row r="646" spans="1:5" ht="12.75">
       <c r="A646" s="10"/>
       <c r="B646" s="10"/>
       <c r="E646" s="11"/>
     </row>
-    <row r="647" spans="1:5" ht="12.75" hidden="1">
+    <row r="647" spans="1:5" ht="12.75">
       <c r="A647" s="10"/>
       <c r="B647" s="10"/>
       <c r="E647" s="11"/>
     </row>
-    <row r="648" spans="1:5" ht="12.75" hidden="1">
+    <row r="648" spans="1:5" ht="12.75">
       <c r="A648" s="10"/>
       <c r="B648" s="10"/>
       <c r="E648" s="11"/>
     </row>
-    <row r="649" spans="1:5" ht="12.75" hidden="1">
+    <row r="649" spans="1:5" ht="12.75">
       <c r="A649" s="10"/>
       <c r="B649" s="10"/>
       <c r="E649" s="11"/>
     </row>
-    <row r="650" spans="1:5" ht="12.75" hidden="1">
+    <row r="650" spans="1:5" ht="12.75">
       <c r="A650" s="10"/>
       <c r="B650" s="10"/>
       <c r="E650" s="11"/>
     </row>
-    <row r="651" spans="1:5" ht="12.75" hidden="1">
+    <row r="651" spans="1:5" ht="12.75">
       <c r="A651" s="10"/>
       <c r="B651" s="10"/>
       <c r="E651" s="11"/>
     </row>
-    <row r="652" spans="1:5" ht="12.75" hidden="1">
+    <row r="652" spans="1:5" ht="12.75">
       <c r="A652" s="10"/>
       <c r="B652" s="10"/>
       <c r="E652" s="11"/>
     </row>
-    <row r="653" spans="1:5" ht="12.75" hidden="1">
+    <row r="653" spans="1:5" ht="12.75">
       <c r="A653" s="10"/>
       <c r="B653" s="10"/>
       <c r="E653" s="11"/>
     </row>
-    <row r="654" spans="1:5" ht="12.75" hidden="1">
+    <row r="654" spans="1:5" ht="12.75">
       <c r="A654" s="10"/>
       <c r="B654" s="10"/>
       <c r="E654" s="11"/>
     </row>
-    <row r="655" spans="1:5" ht="12.75" hidden="1">
+    <row r="655" spans="1:5" ht="12.75">
       <c r="A655" s="10"/>
       <c r="B655" s="10"/>
       <c r="E655" s="11"/>
     </row>
-    <row r="656" spans="1:5" ht="12.75" hidden="1">
+    <row r="656" spans="1:5" ht="12.75">
       <c r="A656" s="10"/>
       <c r="B656" s="10"/>
       <c r="E656" s="11"/>
     </row>
-    <row r="657" spans="1:5" ht="12.75" hidden="1">
+    <row r="657" spans="1:5" ht="12.75">
       <c r="A657" s="10"/>
       <c r="B657" s="10"/>
       <c r="E657" s="11"/>
     </row>
-    <row r="658" spans="1:5" ht="12.75" hidden="1">
+    <row r="658" spans="1:5" ht="12.75">
       <c r="A658" s="10"/>
       <c r="B658" s="10"/>
       <c r="E658" s="11"/>
     </row>
-    <row r="659" spans="1:5" ht="12.75" hidden="1">
+    <row r="659" spans="1:5" ht="12.75">
       <c r="A659" s="10"/>
       <c r="B659" s="10"/>
       <c r="E659" s="11"/>
     </row>
-    <row r="660" spans="1:5" ht="12.75" hidden="1">
+    <row r="660" spans="1:5" ht="12.75">
       <c r="A660" s="10"/>
       <c r="B660" s="10"/>
       <c r="E660" s="11"/>
     </row>
-    <row r="661" spans="1:5" ht="12.75" hidden="1">
+    <row r="661" spans="1:5" ht="12.75">
       <c r="A661" s="10"/>
       <c r="B661" s="10"/>
       <c r="E661" s="11"/>
     </row>
-    <row r="662" spans="1:5" ht="12.75" hidden="1">
+    <row r="662" spans="1:5" ht="12.75">
       <c r="A662" s="10"/>
       <c r="B662" s="10"/>
       <c r="E662" s="11"/>
     </row>
-    <row r="663" spans="1:5" ht="12.75" hidden="1">
+    <row r="663" spans="1:5" ht="12.75">
       <c r="A663" s="10"/>
       <c r="B663" s="10"/>
       <c r="E663" s="11"/>
     </row>
-    <row r="664" spans="1:5" ht="12.75" hidden="1">
+    <row r="664" spans="1:5" ht="12.75">
       <c r="A664" s="10"/>
       <c r="B664" s="10"/>
       <c r="E664" s="11"/>
     </row>
-    <row r="665" spans="1:5" ht="12.75" hidden="1">
+    <row r="665" spans="1:5" ht="12.75">
       <c r="A665" s="10"/>
       <c r="B665" s="10"/>
       <c r="E665" s="11"/>
     </row>
-    <row r="666" spans="1:5" ht="12.75" hidden="1">
+    <row r="666" spans="1:5" ht="12.75">
       <c r="A666" s="10"/>
       <c r="B666" s="10"/>
       <c r="E666" s="11"/>
     </row>
-    <row r="667" spans="1:5" ht="12.75" hidden="1">
+    <row r="667" spans="1:5" ht="12.75">
       <c r="A667" s="10"/>
       <c r="B667" s="10"/>
       <c r="E667" s="11"/>
     </row>
-    <row r="668" spans="1:5" ht="12.75" hidden="1">
+    <row r="668" spans="1:5" ht="12.75">
       <c r="A668" s="10"/>
       <c r="B668" s="10"/>
       <c r="E668" s="11"/>
     </row>
-    <row r="669" spans="1:5" ht="12.75" hidden="1">
+    <row r="669" spans="1:5" ht="12.75">
       <c r="A669" s="10"/>
       <c r="B669" s="10"/>
       <c r="E669" s="11"/>
     </row>
-    <row r="670" spans="1:5" ht="12.75" hidden="1">
+    <row r="670" spans="1:5" ht="12.75">
       <c r="A670" s="10"/>
       <c r="B670" s="10"/>
       <c r="E670" s="11"/>
     </row>
-    <row r="671" spans="1:5" ht="12.75" hidden="1">
+    <row r="671" spans="1:5" ht="12.75">
       <c r="A671" s="10"/>
       <c r="B671" s="10"/>
       <c r="E671" s="11"/>
     </row>
-    <row r="672" spans="1:5" ht="12.75" hidden="1">
+    <row r="672" spans="1:5" ht="12.75">
       <c r="A672" s="10"/>
       <c r="B672" s="10"/>
       <c r="E672" s="11"/>
     </row>
-    <row r="673" spans="1:5" ht="12.75" hidden="1">
+    <row r="673" spans="1:5" ht="12.75">
       <c r="A673" s="10"/>
       <c r="B673" s="10"/>
       <c r="E673" s="11"/>
     </row>
-    <row r="674" spans="1:5" ht="12.75" hidden="1">
+    <row r="674" spans="1:5" ht="12.75">
       <c r="A674" s="10"/>
       <c r="B674" s="10"/>
       <c r="E674" s="11"/>
     </row>
-    <row r="675" spans="1:5" ht="12.75" hidden="1">
+    <row r="675" spans="1:5" ht="12.75">
       <c r="A675" s="10"/>
       <c r="B675" s="10"/>
       <c r="E675" s="11"/>
     </row>
-    <row r="676" spans="1:5" ht="12.75" hidden="1">
+    <row r="676" spans="1:5" ht="12.75">
       <c r="A676" s="10"/>
       <c r="B676" s="10"/>
       <c r="E676" s="11"/>
     </row>
-    <row r="677" spans="1:5" ht="12.75" hidden="1">
+    <row r="677" spans="1:5" ht="12.75">
       <c r="A677" s="10"/>
       <c r="B677" s="10"/>
       <c r="E677" s="11"/>
     </row>
-    <row r="678" spans="1:5" ht="12.75" hidden="1">
+    <row r="678" spans="1:5" ht="12.75">
       <c r="A678" s="10"/>
       <c r="B678" s="10"/>
       <c r="E678" s="11"/>
     </row>
-    <row r="679" spans="1:5" ht="12.75" hidden="1">
+    <row r="679" spans="1:5" ht="12.75">
       <c r="A679" s="10"/>
       <c r="B679" s="10"/>
       <c r="E679" s="11"/>
     </row>
-    <row r="680" spans="1:5" ht="12.75" hidden="1">
+    <row r="680" spans="1:5" ht="12.75">
       <c r="A680" s="10"/>
       <c r="B680" s="10"/>
       <c r="E680" s="11"/>
     </row>
-    <row r="681" spans="1:5" ht="12.75" hidden="1">
+    <row r="681" spans="1:5" ht="12.75">
       <c r="A681" s="10"/>
       <c r="B681" s="10"/>
       <c r="E681" s="11"/>
     </row>
-    <row r="682" spans="1:5" ht="12.75" hidden="1">
+    <row r="682" spans="1:5" ht="12.75">
       <c r="A682" s="10"/>
       <c r="B682" s="10"/>
       <c r="E682" s="11"/>
     </row>
-    <row r="683" spans="1:5" ht="12.75" hidden="1">
+    <row r="683" spans="1:5" ht="12.75">
       <c r="A683" s="10"/>
       <c r="B683" s="10"/>
       <c r="E683" s="11"/>
     </row>
-    <row r="684" spans="1:5" ht="12.75" hidden="1">
+    <row r="684" spans="1:5" ht="12.75">
       <c r="A684" s="10"/>
       <c r="B684" s="10"/>
       <c r="E684" s="11"/>
     </row>
-    <row r="685" spans="1:5" ht="12.75" hidden="1">
+    <row r="685" spans="1:5" ht="12.75">
       <c r="A685" s="10"/>
       <c r="B685" s="10"/>
       <c r="E685" s="11"/>
     </row>
-    <row r="686" spans="1:5" ht="12.75" hidden="1">
+    <row r="686" spans="1:5" ht="12.75">
       <c r="A686" s="10"/>
       <c r="B686" s="10"/>
       <c r="E686" s="11"/>
     </row>
-    <row r="687" spans="1:5" ht="12.75" hidden="1">
+    <row r="687" spans="1:5" ht="12.75">
       <c r="A687" s="10"/>
       <c r="B687" s="10"/>
       <c r="E687" s="11"/>
     </row>
-    <row r="688" spans="1:5" ht="12.75" hidden="1">
+    <row r="688" spans="1:5" ht="12.75">
       <c r="A688" s="10"/>
       <c r="B688" s="10"/>
       <c r="E688" s="11"/>
     </row>
-    <row r="689" spans="1:5" ht="12.75" hidden="1">
+    <row r="689" spans="1:5" ht="12.75">
       <c r="A689" s="10"/>
       <c r="B689" s="10"/>
       <c r="E689" s="11"/>
     </row>
-    <row r="690" spans="1:5" ht="12.75" hidden="1">
+    <row r="690" spans="1:5" ht="12.75">
       <c r="A690" s="10"/>
       <c r="B690" s="10"/>
       <c r="E690" s="11"/>
     </row>
-    <row r="691" spans="1:5" ht="12.75" hidden="1">
+    <row r="691" spans="1:5" ht="12.75">
       <c r="A691" s="10"/>
       <c r="B691" s="10"/>
       <c r="E691" s="11"/>
     </row>
-    <row r="692" spans="1:5" ht="12.75" hidden="1">
+    <row r="692" spans="1:5" ht="12.75">
       <c r="A692" s="10"/>
       <c r="B692" s="10"/>
       <c r="E692" s="11"/>
     </row>
-    <row r="693" spans="1:5" ht="12.75" hidden="1">
+    <row r="693" spans="1:5" ht="12.75">
       <c r="A693" s="10"/>
       <c r="B693" s="10"/>
       <c r="E693" s="11"/>
     </row>
-    <row r="694" spans="1:5" ht="12.75" hidden="1">
+    <row r="694" spans="1:5" ht="12.75">
       <c r="A694" s="10"/>
       <c r="B694" s="10"/>
       <c r="E694" s="11"/>
     </row>
-    <row r="695" spans="1:5" ht="12.75" hidden="1">
+    <row r="695" spans="1:5" ht="12.75">
       <c r="A695" s="10"/>
       <c r="B695" s="10"/>
       <c r="E695" s="11"/>
     </row>
-    <row r="696" spans="1:5" ht="12.75" hidden="1">
+    <row r="696" spans="1:5" ht="12.75">
       <c r="A696" s="10"/>
       <c r="B696" s="10"/>
       <c r="E696" s="11"/>
     </row>
-    <row r="697" spans="1:5" ht="12.75" hidden="1">
+    <row r="697" spans="1:5" ht="12.75">
       <c r="A697" s="10"/>
       <c r="B697" s="10"/>
       <c r="E697" s="11"/>
     </row>
-    <row r="698" spans="1:5" ht="12.75" hidden="1">
+    <row r="698" spans="1:5" ht="12.75">
       <c r="A698" s="10"/>
       <c r="B698" s="10"/>
       <c r="E698" s="11"/>
     </row>
-    <row r="699" spans="1:5" ht="12.75" hidden="1">
+    <row r="699" spans="1:5" ht="12.75">
       <c r="A699" s="10"/>
       <c r="B699" s="10"/>
       <c r="E699" s="11"/>
     </row>
-    <row r="700" spans="1:5" ht="12.75" hidden="1">
+    <row r="700" spans="1:5" ht="12.75">
       <c r="A700" s="10"/>
       <c r="B700" s="10"/>
       <c r="E700" s="11"/>
     </row>
-    <row r="701" spans="1:5" ht="12.75" hidden="1">
+    <row r="701" spans="1:5" ht="12.75">
       <c r="A701" s="10"/>
       <c r="B701" s="10"/>
       <c r="E701" s="11"/>
     </row>
-    <row r="702" spans="1:5" ht="12.75" hidden="1">
+    <row r="702" spans="1:5" ht="12.75">
       <c r="A702" s="10"/>
       <c r="B702" s="10"/>
       <c r="E702" s="11"/>
     </row>
-    <row r="703" spans="1:5" ht="12.75" hidden="1">
+    <row r="703" spans="1:5" ht="12.75">
       <c r="A703" s="10"/>
       <c r="B703" s="10"/>
       <c r="E703" s="11"/>
     </row>
-    <row r="704" spans="1:5" ht="12.75" hidden="1">
+    <row r="704" spans="1:5" ht="12.75">
       <c r="A704" s="10"/>
       <c r="B704" s="10"/>
       <c r="E704" s="11"/>
     </row>
-    <row r="705" spans="1:5" ht="12.75" hidden="1">
+    <row r="705" spans="1:5" ht="12.75">
       <c r="A705" s="10"/>
       <c r="B705" s="10"/>
       <c r="E705" s="11"/>
     </row>
-    <row r="706" spans="1:5" ht="12.75" hidden="1">
+    <row r="706" spans="1:5" ht="12.75">
       <c r="A706" s="10"/>
       <c r="B706" s="10"/>
       <c r="E706" s="11"/>
     </row>
-    <row r="707" spans="1:5" ht="12.75" hidden="1">
+    <row r="707" spans="1:5" ht="12.75">
       <c r="A707" s="10"/>
       <c r="B707" s="10"/>
       <c r="E707" s="11"/>
     </row>
-    <row r="708" spans="1:5" ht="12.75" hidden="1">
+    <row r="708" spans="1:5" ht="12.75">
       <c r="A708" s="10"/>
       <c r="B708" s="10"/>
       <c r="E708" s="11"/>
     </row>
-    <row r="709" spans="1:5" ht="12.75" hidden="1">
+    <row r="709" spans="1:5" ht="12.75">
       <c r="A709" s="10"/>
       <c r="B709" s="10"/>
       <c r="E709" s="11"/>
     </row>
-    <row r="710" spans="1:5" ht="12.75" hidden="1">
+    <row r="710" spans="1:5" ht="12.75">
       <c r="A710" s="10"/>
       <c r="B710" s="10"/>
       <c r="E710" s="11"/>
     </row>
-    <row r="711" spans="1:5" ht="12.75" hidden="1">
+    <row r="711" spans="1:5" ht="12.75">
       <c r="A711" s="10"/>
       <c r="B711" s="10"/>
       <c r="E711" s="11"/>
     </row>
-    <row r="712" spans="1:5" ht="12.75" hidden="1">
+    <row r="712" spans="1:5" ht="12.75">
       <c r="A712" s="10"/>
       <c r="B712" s="10"/>
       <c r="E712" s="11"/>
     </row>
-    <row r="713" spans="1:5" ht="12.75" hidden="1">
+    <row r="713" spans="1:5" ht="12.75">
       <c r="A713" s="10"/>
       <c r="B713" s="10"/>
       <c r="E713" s="11"/>
     </row>
-    <row r="714" spans="1:5" ht="12.75" hidden="1">
+    <row r="714" spans="1:5" ht="12.75">
       <c r="A714" s="10"/>
       <c r="B714" s="10"/>
       <c r="E714" s="11"/>
     </row>
-    <row r="715" spans="1:5" ht="12.75" hidden="1">
+    <row r="715" spans="1:5" ht="12.75">
       <c r="A715" s="10"/>
       <c r="B715" s="10"/>
       <c r="E715" s="11"/>
     </row>
-    <row r="716" spans="1:5" ht="12.75" hidden="1">
+    <row r="716" spans="1:5" ht="12.75">
       <c r="A716" s="10"/>
       <c r="B716" s="10"/>
       <c r="E716" s="11"/>
     </row>
-    <row r="717" spans="1:5" ht="12.75" hidden="1">
+    <row r="717" spans="1:5" ht="12.75">
       <c r="A717" s="10"/>
       <c r="B717" s="10"/>
       <c r="E717" s="11"/>
     </row>
-    <row r="718" spans="1:5" ht="12.75" hidden="1">
+    <row r="718" spans="1:5" ht="12.75">
       <c r="A718" s="10"/>
       <c r="B718" s="10"/>
       <c r="E718" s="11"/>
     </row>
-    <row r="719" spans="1:5" ht="12.75" hidden="1">
+    <row r="719" spans="1:5" ht="12.75">
       <c r="A719" s="10"/>
       <c r="B719" s="10"/>
       <c r="E719" s="11"/>
     </row>
-    <row r="720" spans="1:5" ht="12.75" hidden="1">
+    <row r="720" spans="1:5" ht="12.75">
       <c r="A720" s="10"/>
       <c r="B720" s="10"/>
       <c r="E720" s="11"/>
     </row>
-    <row r="721" spans="1:5" ht="12.75" hidden="1">
+    <row r="721" spans="1:5" ht="12.75">
       <c r="A721" s="10"/>
       <c r="B721" s="10"/>
       <c r="E721" s="11"/>
     </row>
-    <row r="722" spans="1:5" ht="12.75" hidden="1">
+    <row r="722" spans="1:5" ht="12.75">
       <c r="A722" s="10"/>
       <c r="B722" s="10"/>
       <c r="E722" s="11"/>
     </row>
-    <row r="723" spans="1:5" ht="12.75" hidden="1">
+    <row r="723" spans="1:5" ht="12.75">
       <c r="A723" s="10"/>
       <c r="B723" s="10"/>
       <c r="E723" s="11"/>
     </row>
-    <row r="724" spans="1:5" ht="12.75" hidden="1">
+    <row r="724" spans="1:5" ht="12.75">
       <c r="A724" s="10"/>
       <c r="B724" s="10"/>
       <c r="E724" s="11"/>
     </row>
-    <row r="725" spans="1:5" ht="12.75" hidden="1">
+    <row r="725" spans="1:5" ht="12.75">
       <c r="A725" s="10"/>
       <c r="B725" s="10"/>
       <c r="E725" s="11"/>
     </row>
-    <row r="726" spans="1:5" ht="12.75" hidden="1">
+    <row r="726" spans="1:5" ht="12.75">
       <c r="A726" s="10"/>
       <c r="B726" s="10"/>
       <c r="E726" s="11"/>
     </row>
-    <row r="727" spans="1:5" ht="12.75" hidden="1">
+    <row r="727" spans="1:5" ht="12.75">
       <c r="A727" s="10"/>
       <c r="B727" s="10"/>
       <c r="E727" s="11"/>
     </row>
-    <row r="728" spans="1:5" ht="12.75" hidden="1">
+    <row r="728" spans="1:5" ht="12.75">
       <c r="A728" s="10"/>
       <c r="B728" s="10"/>
       <c r="E728" s="11"/>
     </row>
-    <row r="729" spans="1:5" ht="12.75" hidden="1">
+    <row r="729" spans="1:5" ht="12.75">
       <c r="A729" s="10"/>
       <c r="B729" s="10"/>
       <c r="E729" s="11"/>
     </row>
-    <row r="730" spans="1:5" ht="12.75" hidden="1">
+    <row r="730" spans="1:5" ht="12.75">
       <c r="A730" s="10"/>
       <c r="B730" s="10"/>
       <c r="E730" s="11"/>
     </row>
-    <row r="731" spans="1:5" ht="12.75" hidden="1">
+    <row r="731" spans="1:5" ht="12.75">
       <c r="A731" s="10"/>
       <c r="B731" s="10"/>
       <c r="E731" s="11"/>
     </row>
-    <row r="732" spans="1:5" ht="12.75" hidden="1">
+    <row r="732" spans="1:5" ht="12.75">
       <c r="A732" s="10"/>
       <c r="B732" s="10"/>
       <c r="E732" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X732" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:X732" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showDropDown="1" sqref="E3:E106 E111:E732" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes,Maybe"</formula1>

</xml_diff>